<commit_message>
Updating labeling file with new images
</commit_message>
<xml_diff>
--- a/emotiondata.xlsx
+++ b/emotiondata.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27425"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\imran\Desktop\cropped images for focused\new set\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\imran\Desktop\COMP 472\code\a3\biasmitigation\COMP472\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8A636872-329B-4998-ACB4-9B84130B059F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{90C8F02E-DAE3-45A2-9397-15551895C1E3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-28920" yWindow="-5550" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6004" uniqueCount="2402">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6523" uniqueCount="2612">
   <si>
     <t>Number</t>
   </si>
@@ -7231,6 +7231,636 @@
   </si>
   <si>
     <t>Focused/focused-student (12)_cropped.jpg</t>
+  </si>
+  <si>
+    <t>Focused/focused-old-men (4).jpeg</t>
+  </si>
+  <si>
+    <t>Focused/focused-old-men (5).jpeg</t>
+  </si>
+  <si>
+    <t>Focused/focused-old-men (6).jpeg</t>
+  </si>
+  <si>
+    <t>Focused/focused-old-men (7).jpeg</t>
+  </si>
+  <si>
+    <t>Focused/focused-old-men (8).jpeg</t>
+  </si>
+  <si>
+    <t>Focused/focused-old-men (9).jpeg</t>
+  </si>
+  <si>
+    <t>Focused/focused-old-men (10).jpeg</t>
+  </si>
+  <si>
+    <t>Focused/focused-old-men (11).jpeg</t>
+  </si>
+  <si>
+    <t>Focused/focused-old-men (12).jpeg</t>
+  </si>
+  <si>
+    <t>Focused/focused-old-men (13).jpeg</t>
+  </si>
+  <si>
+    <t>Focused/focused-old-men (14).jpeg</t>
+  </si>
+  <si>
+    <t>Focused/focused-old-men (15).jpeg</t>
+  </si>
+  <si>
+    <t>Focused/focused-old-men (16).jpeg</t>
+  </si>
+  <si>
+    <t>Focused/focused-old-men (17).jpeg</t>
+  </si>
+  <si>
+    <t>Focused/focused-old-men (18).jpeg</t>
+  </si>
+  <si>
+    <t>Focused/focused-old-men (19).jpeg</t>
+  </si>
+  <si>
+    <t>Focused/focused-old-men (20).jpeg</t>
+  </si>
+  <si>
+    <t>Focused/focused-old-men (21).jpeg</t>
+  </si>
+  <si>
+    <t>Focused/focused-old-men (22).jpeg</t>
+  </si>
+  <si>
+    <t>Focused/focused-old-men (23).jpeg</t>
+  </si>
+  <si>
+    <t>Focused/focused-old-men (24).jpeg</t>
+  </si>
+  <si>
+    <t>Focused/focused-old-men (25).jpeg</t>
+  </si>
+  <si>
+    <t>Focused/focused-old-men (26).jpeg</t>
+  </si>
+  <si>
+    <t>Focused/focused-old-men (27).jpeg</t>
+  </si>
+  <si>
+    <t>Focused/focused-old-men (28).jpeg</t>
+  </si>
+  <si>
+    <t>Focused/focused-old-men (29).jpeg</t>
+  </si>
+  <si>
+    <t>Focused/focused-old-men (30).jpeg</t>
+  </si>
+  <si>
+    <t>Focused/focused-old-men (31).jpeg</t>
+  </si>
+  <si>
+    <t>Focused/focused-old-men (32).jpeg</t>
+  </si>
+  <si>
+    <t>Focused/focused-old-men (33).jpeg</t>
+  </si>
+  <si>
+    <t>Focused/focused-old-men (34).jpeg</t>
+  </si>
+  <si>
+    <t>Focused/focused-old-men (35).jpeg</t>
+  </si>
+  <si>
+    <t>Focused/focused-old-men (36).jpeg</t>
+  </si>
+  <si>
+    <t>Focused/focused-old-men (37).jpeg</t>
+  </si>
+  <si>
+    <t>Focused/focused-old-men (1).jpeg</t>
+  </si>
+  <si>
+    <t>Focused/focused-old-men (2).jpeg</t>
+  </si>
+  <si>
+    <t>Focused/focused-old-men (3).jpeg</t>
+  </si>
+  <si>
+    <t>https://www.google.ca/search?q=focused+old+men&amp;sca_esv=958dabc01511d05d&amp;sxsrf=ACQVn0_a9dFlN_C49Xi-oGyYiUDkGpwpAg:1713150182105&amp;source=hp&amp;biw=1745&amp;bih=859&amp;ei=5pgcZsqtBNGu5NoP29ui0AQ&amp;iflsig=ANes7DEAAAAAZhym9g0T9xs0XNLokHrNQjFUTD71lmDz&amp;ved=0ahUKEwjKuLLgncOFAxVRF1kFHdutCEoQ4dUDCA8&amp;uact=5&amp;oq=focused+old+men&amp;gs_lp=EgNpbWciD2ZvY3VzZWQgb2xkIG1lbjIEECMYJ0iQElAAWMEPcAB4AJABAJgBZKAB9gmqAQQxNC4xuAEDyAEA-AEBigILZ3dzLXdpei1pbWeYAg-gAqEKwgIIEAAYgAQYsQPCAgUQABiABJgDAJIHBDE0LjGgB7dL&amp;sclient=img&amp;udm=2</t>
+  </si>
+  <si>
+    <t>https://www.google.ca/search?q=focused+old+men&amp;sca_esv=958dabc01511d05d&amp;sxsrf=ACQVn0_a9dFlN_C49Xi-oGyYiUDkGpwpAg:1713150182105&amp;source=hp&amp;biw=1745&amp;bih=859&amp;ei=5pgcZsqtBNGu5NoP29ui0AQ&amp;iflsig=ANes7DEAAAAAZhym9g0T9xs0XNLokHrNQjFUTD71lmDz&amp;ved=0ahUKEwjKuLLgncOFAxVRF1kFHdutCEoQ4dUDCA8&amp;uact=5&amp;oq=focused+old+men&amp;gs_lp=EgNpbWciD2ZvY3VzZWQgb2xkIG1lbjIEECMYJ0iQElAAWMEPcAB4AJABAJgBZKAB9gmqAQQxNC4xuAEDyAEA-AEBigILZ3dzLXdpei1pbWeYAg-gAqEKwgIIEAAYgAQYsQPCAgUQABiABJgDAJIHBDE0LjGgB7dL&amp;sclient=img&amp;udm=3</t>
+  </si>
+  <si>
+    <t>https://www.google.ca/search?q=focused+old+men&amp;sca_esv=958dabc01511d05d&amp;sxsrf=ACQVn0_a9dFlN_C49Xi-oGyYiUDkGpwpAg:1713150182105&amp;source=hp&amp;biw=1745&amp;bih=859&amp;ei=5pgcZsqtBNGu5NoP29ui0AQ&amp;iflsig=ANes7DEAAAAAZhym9g0T9xs0XNLokHrNQjFUTD71lmDz&amp;ved=0ahUKEwjKuLLgncOFAxVRF1kFHdutCEoQ4dUDCA8&amp;uact=5&amp;oq=focused+old+men&amp;gs_lp=EgNpbWciD2ZvY3VzZWQgb2xkIG1lbjIEECMYJ0iQElAAWMEPcAB4AJABAJgBZKAB9gmqAQQxNC4xuAEDyAEA-AEBigILZ3dzLXdpei1pbWeYAg-gAqEKwgIIEAAYgAQYsQPCAgUQABiABJgDAJIHBDE0LjGgB7dL&amp;sclient=img&amp;udm=4</t>
+  </si>
+  <si>
+    <t>https://www.google.ca/search?q=focused+old+men&amp;sca_esv=958dabc01511d05d&amp;sxsrf=ACQVn0_a9dFlN_C49Xi-oGyYiUDkGpwpAg:1713150182105&amp;source=hp&amp;biw=1745&amp;bih=859&amp;ei=5pgcZsqtBNGu5NoP29ui0AQ&amp;iflsig=ANes7DEAAAAAZhym9g0T9xs0XNLokHrNQjFUTD71lmDz&amp;ved=0ahUKEwjKuLLgncOFAxVRF1kFHdutCEoQ4dUDCA8&amp;uact=5&amp;oq=focused+old+men&amp;gs_lp=EgNpbWciD2ZvY3VzZWQgb2xkIG1lbjIEECMYJ0iQElAAWMEPcAB4AJABAJgBZKAB9gmqAQQxNC4xuAEDyAEA-AEBigILZ3dzLXdpei1pbWeYAg-gAqEKwgIIEAAYgAQYsQPCAgUQABiABJgDAJIHBDE0LjGgB7dL&amp;sclient=img&amp;udm=5</t>
+  </si>
+  <si>
+    <t>https://www.google.ca/search?q=focused+old+men&amp;sca_esv=958dabc01511d05d&amp;sxsrf=ACQVn0_a9dFlN_C49Xi-oGyYiUDkGpwpAg:1713150182105&amp;source=hp&amp;biw=1745&amp;bih=859&amp;ei=5pgcZsqtBNGu5NoP29ui0AQ&amp;iflsig=ANes7DEAAAAAZhym9g0T9xs0XNLokHrNQjFUTD71lmDz&amp;ved=0ahUKEwjKuLLgncOFAxVRF1kFHdutCEoQ4dUDCA8&amp;uact=5&amp;oq=focused+old+men&amp;gs_lp=EgNpbWciD2ZvY3VzZWQgb2xkIG1lbjIEECMYJ0iQElAAWMEPcAB4AJABAJgBZKAB9gmqAQQxNC4xuAEDyAEA-AEBigILZ3dzLXdpei1pbWeYAg-gAqEKwgIIEAAYgAQYsQPCAgUQABiABJgDAJIHBDE0LjGgB7dL&amp;sclient=img&amp;udm=6</t>
+  </si>
+  <si>
+    <t>https://www.google.ca/search?q=focused+old+men&amp;sca_esv=958dabc01511d05d&amp;sxsrf=ACQVn0_a9dFlN_C49Xi-oGyYiUDkGpwpAg:1713150182105&amp;source=hp&amp;biw=1745&amp;bih=859&amp;ei=5pgcZsqtBNGu5NoP29ui0AQ&amp;iflsig=ANes7DEAAAAAZhym9g0T9xs0XNLokHrNQjFUTD71lmDz&amp;ved=0ahUKEwjKuLLgncOFAxVRF1kFHdutCEoQ4dUDCA8&amp;uact=5&amp;oq=focused+old+men&amp;gs_lp=EgNpbWciD2ZvY3VzZWQgb2xkIG1lbjIEECMYJ0iQElAAWMEPcAB4AJABAJgBZKAB9gmqAQQxNC4xuAEDyAEA-AEBigILZ3dzLXdpei1pbWeYAg-gAqEKwgIIEAAYgAQYsQPCAgUQABiABJgDAJIHBDE0LjGgB7dL&amp;sclient=img&amp;udm=7</t>
+  </si>
+  <si>
+    <t>https://www.google.ca/search?q=focused+old+men&amp;sca_esv=958dabc01511d05d&amp;sxsrf=ACQVn0_a9dFlN_C49Xi-oGyYiUDkGpwpAg:1713150182105&amp;source=hp&amp;biw=1745&amp;bih=859&amp;ei=5pgcZsqtBNGu5NoP29ui0AQ&amp;iflsig=ANes7DEAAAAAZhym9g0T9xs0XNLokHrNQjFUTD71lmDz&amp;ved=0ahUKEwjKuLLgncOFAxVRF1kFHdutCEoQ4dUDCA8&amp;uact=5&amp;oq=focused+old+men&amp;gs_lp=EgNpbWciD2ZvY3VzZWQgb2xkIG1lbjIEECMYJ0iQElAAWMEPcAB4AJABAJgBZKAB9gmqAQQxNC4xuAEDyAEA-AEBigILZ3dzLXdpei1pbWeYAg-gAqEKwgIIEAAYgAQYsQPCAgUQABiABJgDAJIHBDE0LjGgB7dL&amp;sclient=img&amp;udm=8</t>
+  </si>
+  <si>
+    <t>https://www.google.ca/search?q=focused+old+men&amp;sca_esv=958dabc01511d05d&amp;sxsrf=ACQVn0_a9dFlN_C49Xi-oGyYiUDkGpwpAg:1713150182105&amp;source=hp&amp;biw=1745&amp;bih=859&amp;ei=5pgcZsqtBNGu5NoP29ui0AQ&amp;iflsig=ANes7DEAAAAAZhym9g0T9xs0XNLokHrNQjFUTD71lmDz&amp;ved=0ahUKEwjKuLLgncOFAxVRF1kFHdutCEoQ4dUDCA8&amp;uact=5&amp;oq=focused+old+men&amp;gs_lp=EgNpbWciD2ZvY3VzZWQgb2xkIG1lbjIEECMYJ0iQElAAWMEPcAB4AJABAJgBZKAB9gmqAQQxNC4xuAEDyAEA-AEBigILZ3dzLXdpei1pbWeYAg-gAqEKwgIIEAAYgAQYsQPCAgUQABiABJgDAJIHBDE0LjGgB7dL&amp;sclient=img&amp;udm=9</t>
+  </si>
+  <si>
+    <t>https://www.google.ca/search?q=focused+old+men&amp;sca_esv=958dabc01511d05d&amp;sxsrf=ACQVn0_a9dFlN_C49Xi-oGyYiUDkGpwpAg:1713150182105&amp;source=hp&amp;biw=1745&amp;bih=859&amp;ei=5pgcZsqtBNGu5NoP29ui0AQ&amp;iflsig=ANes7DEAAAAAZhym9g0T9xs0XNLokHrNQjFUTD71lmDz&amp;ved=0ahUKEwjKuLLgncOFAxVRF1kFHdutCEoQ4dUDCA8&amp;uact=5&amp;oq=focused+old+men&amp;gs_lp=EgNpbWciD2ZvY3VzZWQgb2xkIG1lbjIEECMYJ0iQElAAWMEPcAB4AJABAJgBZKAB9gmqAQQxNC4xuAEDyAEA-AEBigILZ3dzLXdpei1pbWeYAg-gAqEKwgIIEAAYgAQYsQPCAgUQABiABJgDAJIHBDE0LjGgB7dL&amp;sclient=img&amp;udm=10</t>
+  </si>
+  <si>
+    <t>https://www.google.ca/search?q=focused+old+men&amp;sca_esv=958dabc01511d05d&amp;sxsrf=ACQVn0_a9dFlN_C49Xi-oGyYiUDkGpwpAg:1713150182105&amp;source=hp&amp;biw=1745&amp;bih=859&amp;ei=5pgcZsqtBNGu5NoP29ui0AQ&amp;iflsig=ANes7DEAAAAAZhym9g0T9xs0XNLokHrNQjFUTD71lmDz&amp;ved=0ahUKEwjKuLLgncOFAxVRF1kFHdutCEoQ4dUDCA8&amp;uact=5&amp;oq=focused+old+men&amp;gs_lp=EgNpbWciD2ZvY3VzZWQgb2xkIG1lbjIEECMYJ0iQElAAWMEPcAB4AJABAJgBZKAB9gmqAQQxNC4xuAEDyAEA-AEBigILZ3dzLXdpei1pbWeYAg-gAqEKwgIIEAAYgAQYsQPCAgUQABiABJgDAJIHBDE0LjGgB7dL&amp;sclient=img&amp;udm=11</t>
+  </si>
+  <si>
+    <t>https://www.google.ca/search?q=focused+old+men&amp;sca_esv=958dabc01511d05d&amp;sxsrf=ACQVn0_a9dFlN_C49Xi-oGyYiUDkGpwpAg:1713150182105&amp;source=hp&amp;biw=1745&amp;bih=859&amp;ei=5pgcZsqtBNGu5NoP29ui0AQ&amp;iflsig=ANes7DEAAAAAZhym9g0T9xs0XNLokHrNQjFUTD71lmDz&amp;ved=0ahUKEwjKuLLgncOFAxVRF1kFHdutCEoQ4dUDCA8&amp;uact=5&amp;oq=focused+old+men&amp;gs_lp=EgNpbWciD2ZvY3VzZWQgb2xkIG1lbjIEECMYJ0iQElAAWMEPcAB4AJABAJgBZKAB9gmqAQQxNC4xuAEDyAEA-AEBigILZ3dzLXdpei1pbWeYAg-gAqEKwgIIEAAYgAQYsQPCAgUQABiABJgDAJIHBDE0LjGgB7dL&amp;sclient=img&amp;udm=12</t>
+  </si>
+  <si>
+    <t>https://www.google.ca/search?q=focused+old+men&amp;sca_esv=958dabc01511d05d&amp;sxsrf=ACQVn0_a9dFlN_C49Xi-oGyYiUDkGpwpAg:1713150182105&amp;source=hp&amp;biw=1745&amp;bih=859&amp;ei=5pgcZsqtBNGu5NoP29ui0AQ&amp;iflsig=ANes7DEAAAAAZhym9g0T9xs0XNLokHrNQjFUTD71lmDz&amp;ved=0ahUKEwjKuLLgncOFAxVRF1kFHdutCEoQ4dUDCA8&amp;uact=5&amp;oq=focused+old+men&amp;gs_lp=EgNpbWciD2ZvY3VzZWQgb2xkIG1lbjIEECMYJ0iQElAAWMEPcAB4AJABAJgBZKAB9gmqAQQxNC4xuAEDyAEA-AEBigILZ3dzLXdpei1pbWeYAg-gAqEKwgIIEAAYgAQYsQPCAgUQABiABJgDAJIHBDE0LjGgB7dL&amp;sclient=img&amp;udm=13</t>
+  </si>
+  <si>
+    <t>https://www.google.ca/search?q=focused+old+men&amp;sca_esv=958dabc01511d05d&amp;sxsrf=ACQVn0_a9dFlN_C49Xi-oGyYiUDkGpwpAg:1713150182105&amp;source=hp&amp;biw=1745&amp;bih=859&amp;ei=5pgcZsqtBNGu5NoP29ui0AQ&amp;iflsig=ANes7DEAAAAAZhym9g0T9xs0XNLokHrNQjFUTD71lmDz&amp;ved=0ahUKEwjKuLLgncOFAxVRF1kFHdutCEoQ4dUDCA8&amp;uact=5&amp;oq=focused+old+men&amp;gs_lp=EgNpbWciD2ZvY3VzZWQgb2xkIG1lbjIEECMYJ0iQElAAWMEPcAB4AJABAJgBZKAB9gmqAQQxNC4xuAEDyAEA-AEBigILZ3dzLXdpei1pbWeYAg-gAqEKwgIIEAAYgAQYsQPCAgUQABiABJgDAJIHBDE0LjGgB7dL&amp;sclient=img&amp;udm=14</t>
+  </si>
+  <si>
+    <t>https://www.google.ca/search?q=focused+old+men&amp;sca_esv=958dabc01511d05d&amp;sxsrf=ACQVn0_a9dFlN_C49Xi-oGyYiUDkGpwpAg:1713150182105&amp;source=hp&amp;biw=1745&amp;bih=859&amp;ei=5pgcZsqtBNGu5NoP29ui0AQ&amp;iflsig=ANes7DEAAAAAZhym9g0T9xs0XNLokHrNQjFUTD71lmDz&amp;ved=0ahUKEwjKuLLgncOFAxVRF1kFHdutCEoQ4dUDCA8&amp;uact=5&amp;oq=focused+old+men&amp;gs_lp=EgNpbWciD2ZvY3VzZWQgb2xkIG1lbjIEECMYJ0iQElAAWMEPcAB4AJABAJgBZKAB9gmqAQQxNC4xuAEDyAEA-AEBigILZ3dzLXdpei1pbWeYAg-gAqEKwgIIEAAYgAQYsQPCAgUQABiABJgDAJIHBDE0LjGgB7dL&amp;sclient=img&amp;udm=15</t>
+  </si>
+  <si>
+    <t>https://www.google.ca/search?q=focused+old+men&amp;sca_esv=958dabc01511d05d&amp;sxsrf=ACQVn0_a9dFlN_C49Xi-oGyYiUDkGpwpAg:1713150182105&amp;source=hp&amp;biw=1745&amp;bih=859&amp;ei=5pgcZsqtBNGu5NoP29ui0AQ&amp;iflsig=ANes7DEAAAAAZhym9g0T9xs0XNLokHrNQjFUTD71lmDz&amp;ved=0ahUKEwjKuLLgncOFAxVRF1kFHdutCEoQ4dUDCA8&amp;uact=5&amp;oq=focused+old+men&amp;gs_lp=EgNpbWciD2ZvY3VzZWQgb2xkIG1lbjIEECMYJ0iQElAAWMEPcAB4AJABAJgBZKAB9gmqAQQxNC4xuAEDyAEA-AEBigILZ3dzLXdpei1pbWeYAg-gAqEKwgIIEAAYgAQYsQPCAgUQABiABJgDAJIHBDE0LjGgB7dL&amp;sclient=img&amp;udm=16</t>
+  </si>
+  <si>
+    <t>https://www.google.ca/search?q=focused+old+men&amp;sca_esv=958dabc01511d05d&amp;sxsrf=ACQVn0_a9dFlN_C49Xi-oGyYiUDkGpwpAg:1713150182105&amp;source=hp&amp;biw=1745&amp;bih=859&amp;ei=5pgcZsqtBNGu5NoP29ui0AQ&amp;iflsig=ANes7DEAAAAAZhym9g0T9xs0XNLokHrNQjFUTD71lmDz&amp;ved=0ahUKEwjKuLLgncOFAxVRF1kFHdutCEoQ4dUDCA8&amp;uact=5&amp;oq=focused+old+men&amp;gs_lp=EgNpbWciD2ZvY3VzZWQgb2xkIG1lbjIEECMYJ0iQElAAWMEPcAB4AJABAJgBZKAB9gmqAQQxNC4xuAEDyAEA-AEBigILZ3dzLXdpei1pbWeYAg-gAqEKwgIIEAAYgAQYsQPCAgUQABiABJgDAJIHBDE0LjGgB7dL&amp;sclient=img&amp;udm=17</t>
+  </si>
+  <si>
+    <t>https://www.google.ca/search?q=focused+old+men&amp;sca_esv=958dabc01511d05d&amp;sxsrf=ACQVn0_a9dFlN_C49Xi-oGyYiUDkGpwpAg:1713150182105&amp;source=hp&amp;biw=1745&amp;bih=859&amp;ei=5pgcZsqtBNGu5NoP29ui0AQ&amp;iflsig=ANes7DEAAAAAZhym9g0T9xs0XNLokHrNQjFUTD71lmDz&amp;ved=0ahUKEwjKuLLgncOFAxVRF1kFHdutCEoQ4dUDCA8&amp;uact=5&amp;oq=focused+old+men&amp;gs_lp=EgNpbWciD2ZvY3VzZWQgb2xkIG1lbjIEECMYJ0iQElAAWMEPcAB4AJABAJgBZKAB9gmqAQQxNC4xuAEDyAEA-AEBigILZ3dzLXdpei1pbWeYAg-gAqEKwgIIEAAYgAQYsQPCAgUQABiABJgDAJIHBDE0LjGgB7dL&amp;sclient=img&amp;udm=18</t>
+  </si>
+  <si>
+    <t>https://www.google.ca/search?q=focused+old+men&amp;sca_esv=958dabc01511d05d&amp;sxsrf=ACQVn0_a9dFlN_C49Xi-oGyYiUDkGpwpAg:1713150182105&amp;source=hp&amp;biw=1745&amp;bih=859&amp;ei=5pgcZsqtBNGu5NoP29ui0AQ&amp;iflsig=ANes7DEAAAAAZhym9g0T9xs0XNLokHrNQjFUTD71lmDz&amp;ved=0ahUKEwjKuLLgncOFAxVRF1kFHdutCEoQ4dUDCA8&amp;uact=5&amp;oq=focused+old+men&amp;gs_lp=EgNpbWciD2ZvY3VzZWQgb2xkIG1lbjIEECMYJ0iQElAAWMEPcAB4AJABAJgBZKAB9gmqAQQxNC4xuAEDyAEA-AEBigILZ3dzLXdpei1pbWeYAg-gAqEKwgIIEAAYgAQYsQPCAgUQABiABJgDAJIHBDE0LjGgB7dL&amp;sclient=img&amp;udm=19</t>
+  </si>
+  <si>
+    <t>https://www.google.ca/search?q=focused+old+men&amp;sca_esv=958dabc01511d05d&amp;sxsrf=ACQVn0_a9dFlN_C49Xi-oGyYiUDkGpwpAg:1713150182105&amp;source=hp&amp;biw=1745&amp;bih=859&amp;ei=5pgcZsqtBNGu5NoP29ui0AQ&amp;iflsig=ANes7DEAAAAAZhym9g0T9xs0XNLokHrNQjFUTD71lmDz&amp;ved=0ahUKEwjKuLLgncOFAxVRF1kFHdutCEoQ4dUDCA8&amp;uact=5&amp;oq=focused+old+men&amp;gs_lp=EgNpbWciD2ZvY3VzZWQgb2xkIG1lbjIEECMYJ0iQElAAWMEPcAB4AJABAJgBZKAB9gmqAQQxNC4xuAEDyAEA-AEBigILZ3dzLXdpei1pbWeYAg-gAqEKwgIIEAAYgAQYsQPCAgUQABiABJgDAJIHBDE0LjGgB7dL&amp;sclient=img&amp;udm=20</t>
+  </si>
+  <si>
+    <t>https://www.google.ca/search?q=focused+old+men&amp;sca_esv=958dabc01511d05d&amp;sxsrf=ACQVn0_a9dFlN_C49Xi-oGyYiUDkGpwpAg:1713150182105&amp;source=hp&amp;biw=1745&amp;bih=859&amp;ei=5pgcZsqtBNGu5NoP29ui0AQ&amp;iflsig=ANes7DEAAAAAZhym9g0T9xs0XNLokHrNQjFUTD71lmDz&amp;ved=0ahUKEwjKuLLgncOFAxVRF1kFHdutCEoQ4dUDCA8&amp;uact=5&amp;oq=focused+old+men&amp;gs_lp=EgNpbWciD2ZvY3VzZWQgb2xkIG1lbjIEECMYJ0iQElAAWMEPcAB4AJABAJgBZKAB9gmqAQQxNC4xuAEDyAEA-AEBigILZ3dzLXdpei1pbWeYAg-gAqEKwgIIEAAYgAQYsQPCAgUQABiABJgDAJIHBDE0LjGgB7dL&amp;sclient=img&amp;udm=21</t>
+  </si>
+  <si>
+    <t>https://www.google.ca/search?q=focused+old+men&amp;sca_esv=958dabc01511d05d&amp;sxsrf=ACQVn0_a9dFlN_C49Xi-oGyYiUDkGpwpAg:1713150182105&amp;source=hp&amp;biw=1745&amp;bih=859&amp;ei=5pgcZsqtBNGu5NoP29ui0AQ&amp;iflsig=ANes7DEAAAAAZhym9g0T9xs0XNLokHrNQjFUTD71lmDz&amp;ved=0ahUKEwjKuLLgncOFAxVRF1kFHdutCEoQ4dUDCA8&amp;uact=5&amp;oq=focused+old+men&amp;gs_lp=EgNpbWciD2ZvY3VzZWQgb2xkIG1lbjIEECMYJ0iQElAAWMEPcAB4AJABAJgBZKAB9gmqAQQxNC4xuAEDyAEA-AEBigILZ3dzLXdpei1pbWeYAg-gAqEKwgIIEAAYgAQYsQPCAgUQABiABJgDAJIHBDE0LjGgB7dL&amp;sclient=img&amp;udm=22</t>
+  </si>
+  <si>
+    <t>https://www.google.ca/search?q=focused+old+men&amp;sca_esv=958dabc01511d05d&amp;sxsrf=ACQVn0_a9dFlN_C49Xi-oGyYiUDkGpwpAg:1713150182105&amp;source=hp&amp;biw=1745&amp;bih=859&amp;ei=5pgcZsqtBNGu5NoP29ui0AQ&amp;iflsig=ANes7DEAAAAAZhym9g0T9xs0XNLokHrNQjFUTD71lmDz&amp;ved=0ahUKEwjKuLLgncOFAxVRF1kFHdutCEoQ4dUDCA8&amp;uact=5&amp;oq=focused+old+men&amp;gs_lp=EgNpbWciD2ZvY3VzZWQgb2xkIG1lbjIEECMYJ0iQElAAWMEPcAB4AJABAJgBZKAB9gmqAQQxNC4xuAEDyAEA-AEBigILZ3dzLXdpei1pbWeYAg-gAqEKwgIIEAAYgAQYsQPCAgUQABiABJgDAJIHBDE0LjGgB7dL&amp;sclient=img&amp;udm=23</t>
+  </si>
+  <si>
+    <t>https://www.google.ca/search?q=focused+old+men&amp;sca_esv=958dabc01511d05d&amp;sxsrf=ACQVn0_a9dFlN_C49Xi-oGyYiUDkGpwpAg:1713150182105&amp;source=hp&amp;biw=1745&amp;bih=859&amp;ei=5pgcZsqtBNGu5NoP29ui0AQ&amp;iflsig=ANes7DEAAAAAZhym9g0T9xs0XNLokHrNQjFUTD71lmDz&amp;ved=0ahUKEwjKuLLgncOFAxVRF1kFHdutCEoQ4dUDCA8&amp;uact=5&amp;oq=focused+old+men&amp;gs_lp=EgNpbWciD2ZvY3VzZWQgb2xkIG1lbjIEECMYJ0iQElAAWMEPcAB4AJABAJgBZKAB9gmqAQQxNC4xuAEDyAEA-AEBigILZ3dzLXdpei1pbWeYAg-gAqEKwgIIEAAYgAQYsQPCAgUQABiABJgDAJIHBDE0LjGgB7dL&amp;sclient=img&amp;udm=24</t>
+  </si>
+  <si>
+    <t>https://www.google.ca/search?q=focused+old+men&amp;sca_esv=958dabc01511d05d&amp;sxsrf=ACQVn0_a9dFlN_C49Xi-oGyYiUDkGpwpAg:1713150182105&amp;source=hp&amp;biw=1745&amp;bih=859&amp;ei=5pgcZsqtBNGu5NoP29ui0AQ&amp;iflsig=ANes7DEAAAAAZhym9g0T9xs0XNLokHrNQjFUTD71lmDz&amp;ved=0ahUKEwjKuLLgncOFAxVRF1kFHdutCEoQ4dUDCA8&amp;uact=5&amp;oq=focused+old+men&amp;gs_lp=EgNpbWciD2ZvY3VzZWQgb2xkIG1lbjIEECMYJ0iQElAAWMEPcAB4AJABAJgBZKAB9gmqAQQxNC4xuAEDyAEA-AEBigILZ3dzLXdpei1pbWeYAg-gAqEKwgIIEAAYgAQYsQPCAgUQABiABJgDAJIHBDE0LjGgB7dL&amp;sclient=img&amp;udm=25</t>
+  </si>
+  <si>
+    <t>https://www.google.ca/search?q=focused+old+men&amp;sca_esv=958dabc01511d05d&amp;sxsrf=ACQVn0_a9dFlN_C49Xi-oGyYiUDkGpwpAg:1713150182105&amp;source=hp&amp;biw=1745&amp;bih=859&amp;ei=5pgcZsqtBNGu5NoP29ui0AQ&amp;iflsig=ANes7DEAAAAAZhym9g0T9xs0XNLokHrNQjFUTD71lmDz&amp;ved=0ahUKEwjKuLLgncOFAxVRF1kFHdutCEoQ4dUDCA8&amp;uact=5&amp;oq=focused+old+men&amp;gs_lp=EgNpbWciD2ZvY3VzZWQgb2xkIG1lbjIEECMYJ0iQElAAWMEPcAB4AJABAJgBZKAB9gmqAQQxNC4xuAEDyAEA-AEBigILZ3dzLXdpei1pbWeYAg-gAqEKwgIIEAAYgAQYsQPCAgUQABiABJgDAJIHBDE0LjGgB7dL&amp;sclient=img&amp;udm=26</t>
+  </si>
+  <si>
+    <t>https://www.google.ca/search?q=focused+old+men&amp;sca_esv=958dabc01511d05d&amp;sxsrf=ACQVn0_a9dFlN_C49Xi-oGyYiUDkGpwpAg:1713150182105&amp;source=hp&amp;biw=1745&amp;bih=859&amp;ei=5pgcZsqtBNGu5NoP29ui0AQ&amp;iflsig=ANes7DEAAAAAZhym9g0T9xs0XNLokHrNQjFUTD71lmDz&amp;ved=0ahUKEwjKuLLgncOFAxVRF1kFHdutCEoQ4dUDCA8&amp;uact=5&amp;oq=focused+old+men&amp;gs_lp=EgNpbWciD2ZvY3VzZWQgb2xkIG1lbjIEECMYJ0iQElAAWMEPcAB4AJABAJgBZKAB9gmqAQQxNC4xuAEDyAEA-AEBigILZ3dzLXdpei1pbWeYAg-gAqEKwgIIEAAYgAQYsQPCAgUQABiABJgDAJIHBDE0LjGgB7dL&amp;sclient=img&amp;udm=27</t>
+  </si>
+  <si>
+    <t>https://www.google.ca/search?q=focused+old+men&amp;sca_esv=958dabc01511d05d&amp;sxsrf=ACQVn0_a9dFlN_C49Xi-oGyYiUDkGpwpAg:1713150182105&amp;source=hp&amp;biw=1745&amp;bih=859&amp;ei=5pgcZsqtBNGu5NoP29ui0AQ&amp;iflsig=ANes7DEAAAAAZhym9g0T9xs0XNLokHrNQjFUTD71lmDz&amp;ved=0ahUKEwjKuLLgncOFAxVRF1kFHdutCEoQ4dUDCA8&amp;uact=5&amp;oq=focused+old+men&amp;gs_lp=EgNpbWciD2ZvY3VzZWQgb2xkIG1lbjIEECMYJ0iQElAAWMEPcAB4AJABAJgBZKAB9gmqAQQxNC4xuAEDyAEA-AEBigILZ3dzLXdpei1pbWeYAg-gAqEKwgIIEAAYgAQYsQPCAgUQABiABJgDAJIHBDE0LjGgB7dL&amp;sclient=img&amp;udm=28</t>
+  </si>
+  <si>
+    <t>https://www.google.ca/search?q=focused+old+men&amp;sca_esv=958dabc01511d05d&amp;sxsrf=ACQVn0_a9dFlN_C49Xi-oGyYiUDkGpwpAg:1713150182105&amp;source=hp&amp;biw=1745&amp;bih=859&amp;ei=5pgcZsqtBNGu5NoP29ui0AQ&amp;iflsig=ANes7DEAAAAAZhym9g0T9xs0XNLokHrNQjFUTD71lmDz&amp;ved=0ahUKEwjKuLLgncOFAxVRF1kFHdutCEoQ4dUDCA8&amp;uact=5&amp;oq=focused+old+men&amp;gs_lp=EgNpbWciD2ZvY3VzZWQgb2xkIG1lbjIEECMYJ0iQElAAWMEPcAB4AJABAJgBZKAB9gmqAQQxNC4xuAEDyAEA-AEBigILZ3dzLXdpei1pbWeYAg-gAqEKwgIIEAAYgAQYsQPCAgUQABiABJgDAJIHBDE0LjGgB7dL&amp;sclient=img&amp;udm=29</t>
+  </si>
+  <si>
+    <t>https://www.google.ca/search?q=focused+old+men&amp;sca_esv=958dabc01511d05d&amp;sxsrf=ACQVn0_a9dFlN_C49Xi-oGyYiUDkGpwpAg:1713150182105&amp;source=hp&amp;biw=1745&amp;bih=859&amp;ei=5pgcZsqtBNGu5NoP29ui0AQ&amp;iflsig=ANes7DEAAAAAZhym9g0T9xs0XNLokHrNQjFUTD71lmDz&amp;ved=0ahUKEwjKuLLgncOFAxVRF1kFHdutCEoQ4dUDCA8&amp;uact=5&amp;oq=focused+old+men&amp;gs_lp=EgNpbWciD2ZvY3VzZWQgb2xkIG1lbjIEECMYJ0iQElAAWMEPcAB4AJABAJgBZKAB9gmqAQQxNC4xuAEDyAEA-AEBigILZ3dzLXdpei1pbWeYAg-gAqEKwgIIEAAYgAQYsQPCAgUQABiABJgDAJIHBDE0LjGgB7dL&amp;sclient=img&amp;udm=30</t>
+  </si>
+  <si>
+    <t>https://www.google.ca/search?q=focused+old+men&amp;sca_esv=958dabc01511d05d&amp;sxsrf=ACQVn0_a9dFlN_C49Xi-oGyYiUDkGpwpAg:1713150182105&amp;source=hp&amp;biw=1745&amp;bih=859&amp;ei=5pgcZsqtBNGu5NoP29ui0AQ&amp;iflsig=ANes7DEAAAAAZhym9g0T9xs0XNLokHrNQjFUTD71lmDz&amp;ved=0ahUKEwjKuLLgncOFAxVRF1kFHdutCEoQ4dUDCA8&amp;uact=5&amp;oq=focused+old+men&amp;gs_lp=EgNpbWciD2ZvY3VzZWQgb2xkIG1lbjIEECMYJ0iQElAAWMEPcAB4AJABAJgBZKAB9gmqAQQxNC4xuAEDyAEA-AEBigILZ3dzLXdpei1pbWeYAg-gAqEKwgIIEAAYgAQYsQPCAgUQABiABJgDAJIHBDE0LjGgB7dL&amp;sclient=img&amp;udm=31</t>
+  </si>
+  <si>
+    <t>https://www.google.ca/search?q=focused+old+men&amp;sca_esv=958dabc01511d05d&amp;sxsrf=ACQVn0_a9dFlN_C49Xi-oGyYiUDkGpwpAg:1713150182105&amp;source=hp&amp;biw=1745&amp;bih=859&amp;ei=5pgcZsqtBNGu5NoP29ui0AQ&amp;iflsig=ANes7DEAAAAAZhym9g0T9xs0XNLokHrNQjFUTD71lmDz&amp;ved=0ahUKEwjKuLLgncOFAxVRF1kFHdutCEoQ4dUDCA8&amp;uact=5&amp;oq=focused+old+men&amp;gs_lp=EgNpbWciD2ZvY3VzZWQgb2xkIG1lbjIEECMYJ0iQElAAWMEPcAB4AJABAJgBZKAB9gmqAQQxNC4xuAEDyAEA-AEBigILZ3dzLXdpei1pbWeYAg-gAqEKwgIIEAAYgAQYsQPCAgUQABiABJgDAJIHBDE0LjGgB7dL&amp;sclient=img&amp;udm=32</t>
+  </si>
+  <si>
+    <t>https://www.google.ca/search?q=focused+old+men&amp;sca_esv=958dabc01511d05d&amp;sxsrf=ACQVn0_a9dFlN_C49Xi-oGyYiUDkGpwpAg:1713150182105&amp;source=hp&amp;biw=1745&amp;bih=859&amp;ei=5pgcZsqtBNGu5NoP29ui0AQ&amp;iflsig=ANes7DEAAAAAZhym9g0T9xs0XNLokHrNQjFUTD71lmDz&amp;ved=0ahUKEwjKuLLgncOFAxVRF1kFHdutCEoQ4dUDCA8&amp;uact=5&amp;oq=focused+old+men&amp;gs_lp=EgNpbWciD2ZvY3VzZWQgb2xkIG1lbjIEECMYJ0iQElAAWMEPcAB4AJABAJgBZKAB9gmqAQQxNC4xuAEDyAEA-AEBigILZ3dzLXdpei1pbWeYAg-gAqEKwgIIEAAYgAQYsQPCAgUQABiABJgDAJIHBDE0LjGgB7dL&amp;sclient=img&amp;udm=33</t>
+  </si>
+  <si>
+    <t>https://www.google.ca/search?q=focused+old+men&amp;sca_esv=958dabc01511d05d&amp;sxsrf=ACQVn0_a9dFlN_C49Xi-oGyYiUDkGpwpAg:1713150182105&amp;source=hp&amp;biw=1745&amp;bih=859&amp;ei=5pgcZsqtBNGu5NoP29ui0AQ&amp;iflsig=ANes7DEAAAAAZhym9g0T9xs0XNLokHrNQjFUTD71lmDz&amp;ved=0ahUKEwjKuLLgncOFAxVRF1kFHdutCEoQ4dUDCA8&amp;uact=5&amp;oq=focused+old+men&amp;gs_lp=EgNpbWciD2ZvY3VzZWQgb2xkIG1lbjIEECMYJ0iQElAAWMEPcAB4AJABAJgBZKAB9gmqAQQxNC4xuAEDyAEA-AEBigILZ3dzLXdpei1pbWeYAg-gAqEKwgIIEAAYgAQYsQPCAgUQABiABJgDAJIHBDE0LjGgB7dL&amp;sclient=img&amp;udm=34</t>
+  </si>
+  <si>
+    <t>https://www.google.ca/search?q=focused+old+men&amp;sca_esv=958dabc01511d05d&amp;sxsrf=ACQVn0_a9dFlN_C49Xi-oGyYiUDkGpwpAg:1713150182105&amp;source=hp&amp;biw=1745&amp;bih=859&amp;ei=5pgcZsqtBNGu5NoP29ui0AQ&amp;iflsig=ANes7DEAAAAAZhym9g0T9xs0XNLokHrNQjFUTD71lmDz&amp;ved=0ahUKEwjKuLLgncOFAxVRF1kFHdutCEoQ4dUDCA8&amp;uact=5&amp;oq=focused+old+men&amp;gs_lp=EgNpbWciD2ZvY3VzZWQgb2xkIG1lbjIEECMYJ0iQElAAWMEPcAB4AJABAJgBZKAB9gmqAQQxNC4xuAEDyAEA-AEBigILZ3dzLXdpei1pbWeYAg-gAqEKwgIIEAAYgAQYsQPCAgUQABiABJgDAJIHBDE0LjGgB7dL&amp;sclient=img&amp;udm=35</t>
+  </si>
+  <si>
+    <t>https://www.google.ca/search?q=focused+old+men&amp;sca_esv=958dabc01511d05d&amp;sxsrf=ACQVn0_a9dFlN_C49Xi-oGyYiUDkGpwpAg:1713150182105&amp;source=hp&amp;biw=1745&amp;bih=859&amp;ei=5pgcZsqtBNGu5NoP29ui0AQ&amp;iflsig=ANes7DEAAAAAZhym9g0T9xs0XNLokHrNQjFUTD71lmDz&amp;ved=0ahUKEwjKuLLgncOFAxVRF1kFHdutCEoQ4dUDCA8&amp;uact=5&amp;oq=focused+old+men&amp;gs_lp=EgNpbWciD2ZvY3VzZWQgb2xkIG1lbjIEECMYJ0iQElAAWMEPcAB4AJABAJgBZKAB9gmqAQQxNC4xuAEDyAEA-AEBigILZ3dzLXdpei1pbWeYAg-gAqEKwgIIEAAYgAQYsQPCAgUQABiABJgDAJIHBDE0LjGgB7dL&amp;sclient=img&amp;udm=36</t>
+  </si>
+  <si>
+    <t>https://www.google.ca/search?q=focused+old+men&amp;sca_esv=958dabc01511d05d&amp;sxsrf=ACQVn0_a9dFlN_C49Xi-oGyYiUDkGpwpAg:1713150182105&amp;source=hp&amp;biw=1745&amp;bih=859&amp;ei=5pgcZsqtBNGu5NoP29ui0AQ&amp;iflsig=ANes7DEAAAAAZhym9g0T9xs0XNLokHrNQjFUTD71lmDz&amp;ved=0ahUKEwjKuLLgncOFAxVRF1kFHdutCEoQ4dUDCA8&amp;uact=5&amp;oq=focused+old+men&amp;gs_lp=EgNpbWciD2ZvY3VzZWQgb2xkIG1lbjIEECMYJ0iQElAAWMEPcAB4AJABAJgBZKAB9gmqAQQxNC4xuAEDyAEA-AEBigILZ3dzLXdpei1pbWeYAg-gAqEKwgIIEAAYgAQYsQPCAgUQABiABJgDAJIHBDE0LjGgB7dL&amp;sclient=img&amp;udm=37</t>
+  </si>
+  <si>
+    <t>https://www.google.ca/search?q=focused+old+men&amp;sca_esv=958dabc01511d05d&amp;sxsrf=ACQVn0_a9dFlN_C49Xi-oGyYiUDkGpwpAg:1713150182105&amp;source=hp&amp;biw=1745&amp;bih=859&amp;ei=5pgcZsqtBNGu5NoP29ui0AQ&amp;iflsig=ANes7DEAAAAAZhym9g0T9xs0XNLokHrNQjFUTD71lmDz&amp;ved=0ahUKEwjKuLLgncOFAxVRF1kFHdutCEoQ4dUDCA8&amp;uact=5&amp;oq=focused+old+men&amp;gs_lp=EgNpbWciD2ZvY3VzZWQgb2xkIG1lbjIEECMYJ0iQElAAWMEPcAB4AJABAJgBZKAB9gmqAQQxNC4xuAEDyAEA-AEBigILZ3dzLXdpei1pbWeYAg-gAqEKwgIIEAAYgAQYsQPCAgUQABiABJgDAJIHBDE0LjGgB7dL&amp;sclient=img&amp;udm=38</t>
+  </si>
+  <si>
+    <t>Happy/cropped_emotions.271961.png</t>
+  </si>
+  <si>
+    <t>Happy/cropped_emotions.271982.png</t>
+  </si>
+  <si>
+    <t>Happy/cropped_emotions.271984.png</t>
+  </si>
+  <si>
+    <t>Happy/cropped_emotions.271994.png</t>
+  </si>
+  <si>
+    <t>Happy/cropped_emotions.272014.png</t>
+  </si>
+  <si>
+    <t>Happy/cropped_emotions.272017.png</t>
+  </si>
+  <si>
+    <t>Happy/cropped_emotions.272018.png</t>
+  </si>
+  <si>
+    <t>Happy/cropped_emotions.272024.png</t>
+  </si>
+  <si>
+    <t>Happy/cropped_emotions.374489.png</t>
+  </si>
+  <si>
+    <t>Happy/cropped_emotions.398493.png</t>
+  </si>
+  <si>
+    <t>Happy/cropped_emotions.398521.png</t>
+  </si>
+  <si>
+    <t>Happy/cropped_emotions.398537.png</t>
+  </si>
+  <si>
+    <t>Happy/cropped_emotions.398572.png</t>
+  </si>
+  <si>
+    <t>Happy/cropped_emotions.398650.png</t>
+  </si>
+  <si>
+    <t>Happy/cropped_emotions.418294.png</t>
+  </si>
+  <si>
+    <t>Happy/cropped_emotions.418302.png</t>
+  </si>
+  <si>
+    <t>Happy/cropped_emotions.418358.png</t>
+  </si>
+  <si>
+    <t>Happy/cropped_emotions.418523.png</t>
+  </si>
+  <si>
+    <t>Happy/cropped_emotions.505732.png</t>
+  </si>
+  <si>
+    <t>Happy/cropped_emotions.505734.png</t>
+  </si>
+  <si>
+    <t>Happy/cropped_emotions.505736.png</t>
+  </si>
+  <si>
+    <t>Happy/cropped_emotions.505739.png</t>
+  </si>
+  <si>
+    <t>Happy/cropped_emotions.505818.png</t>
+  </si>
+  <si>
+    <t>Happy/cropped_emotions.505830.png</t>
+  </si>
+  <si>
+    <t>Happy/cropped_emotions.505835.png</t>
+  </si>
+  <si>
+    <t>Happy/cropped_emotions.505840.png</t>
+  </si>
+  <si>
+    <t>Happy/cropped_emotions.505878.png</t>
+  </si>
+  <si>
+    <t>Happy/cropped_emotions.505899.png</t>
+  </si>
+  <si>
+    <t>Happy/cropped_emotions.505913.png</t>
+  </si>
+  <si>
+    <t>Happy/cropped_emotions.505927.png</t>
+  </si>
+  <si>
+    <t>Happy/cropped_emotions.505938.png</t>
+  </si>
+  <si>
+    <t>Happy/cropped_emotions.506000.png</t>
+  </si>
+  <si>
+    <t>Happy/cropped_emotions.506022.png</t>
+  </si>
+  <si>
+    <t>Happy/cropped_emotions.506038.png</t>
+  </si>
+  <si>
+    <t>Happy/cropped_emotions.506063.png</t>
+  </si>
+  <si>
+    <t>Happy/cropped_emotions.506077.png</t>
+  </si>
+  <si>
+    <t>Happy/cropped_emotions.506088.png</t>
+  </si>
+  <si>
+    <t>Happy/cropped_emotions.506109.png</t>
+  </si>
+  <si>
+    <t>Happy/cropped_emotions.506130.png</t>
+  </si>
+  <si>
+    <t>Happy/cropped_emotions.506156.png</t>
+  </si>
+  <si>
+    <t>Happy/cropped_emotions.506194.png</t>
+  </si>
+  <si>
+    <t>Happy/cropped_emotions.506208.png</t>
+  </si>
+  <si>
+    <t>Happy/cropped_emotions.506229.png</t>
+  </si>
+  <si>
+    <t>Happy/cropped_emotions.568075.png</t>
+  </si>
+  <si>
+    <t>Happy/cropped_emotions.569060.png</t>
+  </si>
+  <si>
+    <t>Happy/3ac4ae1f73b7b3b7abcaa69dd5185a70dda5a860cae4997d020c494d.jpg</t>
+  </si>
+  <si>
+    <t>Happy/3bef83da9c47258e221f84ee3ec1ab808bb7374273fd0a28471dd108.jpg</t>
+  </si>
+  <si>
+    <t>Happy/cropped_emotions.271879.png</t>
+  </si>
+  <si>
+    <t>Happy/cropped_emotions.271919.png</t>
+  </si>
+  <si>
+    <t>Happy/cropped_emotions.271938.png</t>
+  </si>
+  <si>
+    <t>Neutral/00b6d6cccd570d1ac06219aec65fb4c667760e645db8e074c7dac0adf.JPG</t>
+  </si>
+  <si>
+    <t>Neutral/00b1478ebfd81ceaf04642908a07ab9c1ecd07f2cf305a37a9dcf667f.jpg</t>
+  </si>
+  <si>
+    <t>Neutral/00b029289cb05cbfec7eaa149c85088cb0151d7646c083be95ce731ff(1).jpg</t>
+  </si>
+  <si>
+    <t>Neutral/00b029289cb05cbfec7eaa149c85088cb0151d7646c083be95ce731ff.jpg</t>
+  </si>
+  <si>
+    <t>Neutral/00c1df747a813a396df2bcf055179d5db294f44943b5d1415b360080f.jpg</t>
+  </si>
+  <si>
+    <t>Neutral/00c44b9366ba6ec6e8014d7772883ffe4e7f643ba51c5b08b8ab1b6cf.jpg</t>
+  </si>
+  <si>
+    <t>Neutral/00caab9df8103ee25aaaaed6aaa12bb03ffb10b02f7e652bb75b96dbf.jpg</t>
+  </si>
+  <si>
+    <t>Neutral/00e6b0695fde9450295b55a3d1600971c62dd6dac45b0a67a53780a6f.jpg</t>
+  </si>
+  <si>
+    <t>Neutral/00e00402a0af0c9fefe27fbc6db7c669d8ad2c899f157bd74c8a98f7f.jpg</t>
+  </si>
+  <si>
+    <t>Neutral/0dd2e60fb7fe4a1de206b73e2cea3e7ca213a27a60ab646aab830645f.jpg</t>
+  </si>
+  <si>
+    <t>Neutral/0e00ab3ca7e8f7ab6c4426e4cf00e8255d623191cc14b380dd36cad1f.JPG</t>
+  </si>
+  <si>
+    <t>Neutral/0e0e00b630603ffbf19b63978db0b1d6e66a0f0ad1e24bb9db5794b2f.jpg</t>
+  </si>
+  <si>
+    <t>Neutral/0e3dec55c2e969bb240309e613dc0b9497555ff6412a2b2e2eeae5acf.jpg</t>
+  </si>
+  <si>
+    <t>Neutral/0e3e010154b31bd9fb522c12284019fa0d6514bc5cc8ca4169cbd0abf.jpg</t>
+  </si>
+  <si>
+    <t>Neutral/0e4b3f20fffde314cbdc8584dcece95ac8686e1ffb8badfbc8861335f.jpg</t>
+  </si>
+  <si>
+    <t>Neutral/0e7fb831310ae9066192c5abfc3de2264f64644daa9462457d868297f.jpg</t>
+  </si>
+  <si>
+    <t>Neutral/0e8eff3d7a42b3f7a7fbe237fbd114c377a25794e6b0bbb5016582fbf.jpg</t>
+  </si>
+  <si>
+    <t>Neutral/0e8f9b9b5590bdc615dca2a0fe3bc8313c550f8a7a31f7a47e0b52b6f.jpg</t>
+  </si>
+  <si>
+    <t>Neutral/0e9d0e639c377ce3c0018b49d800ead849fb7d8ef421de000e54418ff.jpg</t>
+  </si>
+  <si>
+    <t>Neutral/0e049bbb0ff80b3fb9377c1c81b296283ce394fe75541c083b126081f.jpg</t>
+  </si>
+  <si>
+    <t>Neutral/0e66ce9b10ce90f53690ad158d22294e415febbaae8daaecb58e3cc8f.jpg</t>
+  </si>
+  <si>
+    <t>Neutral/0e66f97ec58a2c4c1136b67cc2137202c453bd82a35f930d736732bbf.jpg</t>
+  </si>
+  <si>
+    <t>Neutral/0e340f919597555f0108236b237e5992642b37101724db5eb020a15ef.jpg</t>
+  </si>
+  <si>
+    <t>Neutral/0e422ab478f80e65575016161c766c07fe552124eddcbf29f33ca09ef.jpeg</t>
+  </si>
+  <si>
+    <t>Neutral/0e490a244d8b0a8f7457ddefaa6cf02dbe5efff5ad475c5bf320d55bf.jpg</t>
+  </si>
+  <si>
+    <t>Neutral/0e1566fa10d9f2bc65897507fbdb42efa828be4f103fe42e96fd5a08f.jpg</t>
+  </si>
+  <si>
+    <t>Neutral/0e2373cec22b9e0399f52cbe49298a04edb8ded86b60072955e53f29f.jpg</t>
+  </si>
+  <si>
+    <t>Neutral/0e3734c79f465dab7c6ce7aade4503b0ab1ec7d3b95e35c7cb142e77f.jpg</t>
+  </si>
+  <si>
+    <t>Neutral/0e4362eb85a72ab281ec91d53788218c464a01401f6a42246f992baaf.jpg</t>
+  </si>
+  <si>
+    <t>Neutral/0ea51d1e4af8d16291b491ec7b7216e054db82036e0618178fc89b60f.jpg</t>
+  </si>
+  <si>
+    <t>Neutral/0ea947e69ebc942aac0cd6cd25229346d1ba99bc0d0cef3315a3cc69f.jpg</t>
+  </si>
+  <si>
+    <t>Neutral/0eacb2a1ba776de9aeb82a3a76794f7a60523a10393d9afba35b14b7f.jpg</t>
+  </si>
+  <si>
+    <t>Neutral/0eaf9fc537c0aa278e961af3efe2781a62676de528f64b1fd5210b2bf.jpg</t>
+  </si>
+  <si>
+    <t>Neutral/0eb14b219e78149f185a335a55a430bda498ee7701f000d5637dcfc3f.jpg</t>
+  </si>
+  <si>
+    <t>Neutral/0ecd719e43d6e6eea6514996ddaf716d961550da12be37ef33c46aa1f.jpg</t>
+  </si>
+  <si>
+    <t>Neutral/0edc1764fb1a6b4a4085a22752ad692b1b3b4bed2e83ab84a54d0c24f.jpg</t>
+  </si>
+  <si>
+    <t>Neutral/0eff073c442b6d02129e5114025b794b1bbc6ddc98c1bc09a46691dcf.jpg</t>
+  </si>
+  <si>
+    <t>Neutral/0f0e8c18dc887d68dc91158bcdfcee726314d9aa021fb2de44dc528df.jpg</t>
+  </si>
+  <si>
+    <t>Neutral/0f04eabba1c614a6955491b51ea9c2dbec33b71f25450be53fc5a6f0f.jpg</t>
+  </si>
+  <si>
+    <t>Neutral/0f8ade6beea6d913e062b031cba379eea9e11563c8021707376da5c7f.jpg</t>
+  </si>
+  <si>
+    <t>Neutral/0f8d2e238b9a1b90fc1c48958650665578e1e81dfd3e353d568ed6b1f.jpg</t>
+  </si>
+  <si>
+    <t>Neutral/0f8d907a3ebc9cb7bd17c9e07e122da7f05f51060c69fa730abe9004f.jpg</t>
+  </si>
+  <si>
+    <t>Neutral/0f8da162bca0eb129ac058960a1549c4071ac671f775e4d39290302cf.jpg</t>
+  </si>
+  <si>
+    <t>Neutral/0f50be764a33c448184017a9e47d9d71b210bf9f4e2adabb31ae2b34f.jpeg</t>
+  </si>
+  <si>
+    <t>Neutral/0f92f5dbe973229558c605b9edc276216a6f21f3f2a8f725daeb7c8df.jpg</t>
+  </si>
+  <si>
+    <t>Neutral/0f113f6b11d546cd9af920d7732385e1a38b79c18598f18444765f71f.jpg</t>
+  </si>
+  <si>
+    <t>Neutral/0f245ee5f54722257a02d1d773526a93440e085f1e234bb4913f01c7f.jpg</t>
+  </si>
+  <si>
+    <t>Neutral/000adf1bba31e39ce59b5222c82c89d61536a6c8bf1dd8ac50d99b3cf.jpg</t>
+  </si>
+  <si>
+    <t>Neutral/00a1a2bd781f3a4e74c177c0bea2e25c8e15be72cb6a1b878bc6685af.jpg</t>
+  </si>
+  <si>
+    <t>Neutral/00aa7706762bdbd7f32b1436a523bcf7be50855733a192af27a0cebef.jpg</t>
+  </si>
+  <si>
+    <t>Suprised/1fa9bc30ca4aba6504eb114c9cff30687c2b727ab909ce2cda8faa6f~12fffff.jpg</t>
+  </si>
+  <si>
+    <t>Suprised/cropped_emotions.99989~12fffff.png</t>
+  </si>
+  <si>
+    <t>Suprised/cropped_emotions.99994~12fffff.png</t>
+  </si>
+  <si>
+    <t>Suprised/cropped_emotions.100019~12fffff.png</t>
+  </si>
+  <si>
+    <t>Suprised/cropped_emotions.100033~12fffff.png</t>
+  </si>
+  <si>
+    <t>Suprised/cropped_emotions.100080~12fffff.png</t>
+  </si>
+  <si>
+    <t>Suprised/cropped_emotions.100084~12fffff.png</t>
+  </si>
+  <si>
+    <t>Suprised/cropped_emotions.100112~12fffff.png</t>
+  </si>
+  <si>
+    <t>Suprised/cropped_emotions.100126~12fffff.png</t>
+  </si>
+  <si>
+    <t>Suprised/cropped_emotions.100143~12fffff.png</t>
+  </si>
+  <si>
+    <t>Suprised/cropped_emotions.100147~12fffff.png</t>
+  </si>
+  <si>
+    <t>Suprised/cropped_emotions.100163~12fffff.png</t>
+  </si>
+  <si>
+    <t>Suprised/cropped_emotions.100171~12fffff.png</t>
+  </si>
+  <si>
+    <t>Suprised/cropped_emotions.100183~12fffff.png</t>
+  </si>
+  <si>
+    <t>Suprised/cropped_emotions.100201~12fffff.png</t>
+  </si>
+  <si>
+    <t>Suprised/cropped_emotions.100220~12fffff.png</t>
+  </si>
+  <si>
+    <t>Suprised/cropped_emotions.100232~12fffff.png</t>
+  </si>
+  <si>
+    <t>Suprised/cropped_emotions.100238~12fffff.png</t>
+  </si>
+  <si>
+    <t>Suprised/cropped_emotions.100244~12fffff.png</t>
+  </si>
+  <si>
+    <t>Suprised/cropped_emotions.100245~12fffff.png</t>
+  </si>
+  <si>
+    <t>Suprised/cropped_emotions.100275~12fffff.png</t>
+  </si>
+  <si>
+    <t>Suprised/cropped_emotions.100279~12fffff.png</t>
+  </si>
+  <si>
+    <t>Suprised/cropped_emotions.260089~12fffff.png</t>
+  </si>
+  <si>
+    <t>Suprised/cropped_emotions.260316~12fffff.png</t>
+  </si>
+  <si>
+    <t>Suprised/cropped_emotions.260987~12fffff.png</t>
+  </si>
+  <si>
+    <t>Suprised/cropped_emotions.261011~12fffff.png</t>
+  </si>
+  <si>
+    <t>Suprised/cropped_emotions.261111~12fffff.png</t>
+  </si>
+  <si>
+    <t>Suprised/cropped_emotions.261291~12fffff.png</t>
+  </si>
+  <si>
+    <t>Suprised/cropped_emotions.262101~12fffff.png</t>
+  </si>
+  <si>
+    <t>Suprised/cropped_emotions.262286~12fffff.png</t>
+  </si>
+  <si>
+    <t>Suprised/cropped_emotions.262564~12fffff.png</t>
+  </si>
+  <si>
+    <t>Suprised/0af47fdcd18ee87deeae0a2606625218e257ac1331e4ef75181431be~12fffff.jpeg</t>
+  </si>
+  <si>
+    <t>Suprised/0af78628cb17d8d509db190e4d400489afebaa4ff1e9bc92a817b8cd~12fffff.jpg</t>
+  </si>
+  <si>
+    <t>Suprised/0bff78216369acf844f5fe5a79262e3de0b03aae090cdc92f9d5c270~12fffff.jpg</t>
+  </si>
+  <si>
+    <t>Suprised/1e2e7ca47b324992d0068a1376b31c5bae777fa73751636689b6e8fd~12fffff.jpg</t>
+  </si>
+  <si>
+    <t>Suprised/1e9103d3608a4301872a90b9b53861012d9f1c7a0ea17f3a496e8d50~12fffff.jpg</t>
   </si>
 </sst>
 </file>
@@ -7554,10 +8184,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D2001"/>
+  <dimension ref="A1:D2174"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A1984" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="B2009" sqref="B2009"/>
+    <sheetView tabSelected="1" topLeftCell="A1983" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="I2156" sqref="I2156"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -35581,6 +36211,2428 @@
         <v>1901</v>
       </c>
     </row>
+    <row r="2002" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A2002">
+        <v>2001</v>
+      </c>
+      <c r="B2002" t="s">
+        <v>2402</v>
+      </c>
+      <c r="C2002" t="s">
+        <v>1508</v>
+      </c>
+      <c r="D2002" t="s">
+        <v>2439</v>
+      </c>
+    </row>
+    <row r="2003" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A2003">
+        <v>2002</v>
+      </c>
+      <c r="B2003" t="s">
+        <v>2403</v>
+      </c>
+      <c r="C2003" t="s">
+        <v>1508</v>
+      </c>
+      <c r="D2003" t="s">
+        <v>2440</v>
+      </c>
+    </row>
+    <row r="2004" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A2004">
+        <v>2003</v>
+      </c>
+      <c r="B2004" t="s">
+        <v>2404</v>
+      </c>
+      <c r="C2004" t="s">
+        <v>1508</v>
+      </c>
+      <c r="D2004" t="s">
+        <v>2441</v>
+      </c>
+    </row>
+    <row r="2005" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A2005">
+        <v>2004</v>
+      </c>
+      <c r="B2005" t="s">
+        <v>2405</v>
+      </c>
+      <c r="C2005" t="s">
+        <v>1508</v>
+      </c>
+      <c r="D2005" t="s">
+        <v>2442</v>
+      </c>
+    </row>
+    <row r="2006" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A2006">
+        <v>2005</v>
+      </c>
+      <c r="B2006" t="s">
+        <v>2406</v>
+      </c>
+      <c r="C2006" t="s">
+        <v>1508</v>
+      </c>
+      <c r="D2006" t="s">
+        <v>2443</v>
+      </c>
+    </row>
+    <row r="2007" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A2007">
+        <v>2006</v>
+      </c>
+      <c r="B2007" t="s">
+        <v>2407</v>
+      </c>
+      <c r="C2007" t="s">
+        <v>1508</v>
+      </c>
+      <c r="D2007" t="s">
+        <v>2444</v>
+      </c>
+    </row>
+    <row r="2008" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A2008">
+        <v>2007</v>
+      </c>
+      <c r="B2008" t="s">
+        <v>2408</v>
+      </c>
+      <c r="C2008" t="s">
+        <v>1508</v>
+      </c>
+      <c r="D2008" t="s">
+        <v>2445</v>
+      </c>
+    </row>
+    <row r="2009" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A2009">
+        <v>2008</v>
+      </c>
+      <c r="B2009" t="s">
+        <v>2409</v>
+      </c>
+      <c r="C2009" t="s">
+        <v>1508</v>
+      </c>
+      <c r="D2009" t="s">
+        <v>2446</v>
+      </c>
+    </row>
+    <row r="2010" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A2010">
+        <v>2009</v>
+      </c>
+      <c r="B2010" t="s">
+        <v>2410</v>
+      </c>
+      <c r="C2010" t="s">
+        <v>1508</v>
+      </c>
+      <c r="D2010" t="s">
+        <v>2447</v>
+      </c>
+    </row>
+    <row r="2011" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A2011">
+        <v>2010</v>
+      </c>
+      <c r="B2011" t="s">
+        <v>2411</v>
+      </c>
+      <c r="C2011" t="s">
+        <v>1508</v>
+      </c>
+      <c r="D2011" t="s">
+        <v>2448</v>
+      </c>
+    </row>
+    <row r="2012" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A2012">
+        <v>2011</v>
+      </c>
+      <c r="B2012" t="s">
+        <v>2412</v>
+      </c>
+      <c r="C2012" t="s">
+        <v>1508</v>
+      </c>
+      <c r="D2012" t="s">
+        <v>2449</v>
+      </c>
+    </row>
+    <row r="2013" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A2013">
+        <v>2012</v>
+      </c>
+      <c r="B2013" t="s">
+        <v>2413</v>
+      </c>
+      <c r="C2013" t="s">
+        <v>1508</v>
+      </c>
+      <c r="D2013" t="s">
+        <v>2450</v>
+      </c>
+    </row>
+    <row r="2014" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A2014">
+        <v>2013</v>
+      </c>
+      <c r="B2014" t="s">
+        <v>2414</v>
+      </c>
+      <c r="C2014" t="s">
+        <v>1508</v>
+      </c>
+      <c r="D2014" t="s">
+        <v>2451</v>
+      </c>
+    </row>
+    <row r="2015" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A2015">
+        <v>2014</v>
+      </c>
+      <c r="B2015" t="s">
+        <v>2415</v>
+      </c>
+      <c r="C2015" t="s">
+        <v>1508</v>
+      </c>
+      <c r="D2015" t="s">
+        <v>2452</v>
+      </c>
+    </row>
+    <row r="2016" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A2016">
+        <v>2015</v>
+      </c>
+      <c r="B2016" t="s">
+        <v>2416</v>
+      </c>
+      <c r="C2016" t="s">
+        <v>1508</v>
+      </c>
+      <c r="D2016" t="s">
+        <v>2453</v>
+      </c>
+    </row>
+    <row r="2017" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A2017">
+        <v>2016</v>
+      </c>
+      <c r="B2017" t="s">
+        <v>2417</v>
+      </c>
+      <c r="C2017" t="s">
+        <v>1508</v>
+      </c>
+      <c r="D2017" t="s">
+        <v>2454</v>
+      </c>
+    </row>
+    <row r="2018" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A2018">
+        <v>2017</v>
+      </c>
+      <c r="B2018" t="s">
+        <v>2418</v>
+      </c>
+      <c r="C2018" t="s">
+        <v>1508</v>
+      </c>
+      <c r="D2018" t="s">
+        <v>2455</v>
+      </c>
+    </row>
+    <row r="2019" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A2019">
+        <v>2018</v>
+      </c>
+      <c r="B2019" t="s">
+        <v>2419</v>
+      </c>
+      <c r="C2019" t="s">
+        <v>1508</v>
+      </c>
+      <c r="D2019" t="s">
+        <v>2456</v>
+      </c>
+    </row>
+    <row r="2020" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A2020">
+        <v>2019</v>
+      </c>
+      <c r="B2020" t="s">
+        <v>2420</v>
+      </c>
+      <c r="C2020" t="s">
+        <v>1508</v>
+      </c>
+      <c r="D2020" t="s">
+        <v>2457</v>
+      </c>
+    </row>
+    <row r="2021" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A2021">
+        <v>2020</v>
+      </c>
+      <c r="B2021" t="s">
+        <v>2421</v>
+      </c>
+      <c r="C2021" t="s">
+        <v>1508</v>
+      </c>
+      <c r="D2021" t="s">
+        <v>2458</v>
+      </c>
+    </row>
+    <row r="2022" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A2022">
+        <v>2021</v>
+      </c>
+      <c r="B2022" t="s">
+        <v>2422</v>
+      </c>
+      <c r="C2022" t="s">
+        <v>1508</v>
+      </c>
+      <c r="D2022" t="s">
+        <v>2459</v>
+      </c>
+    </row>
+    <row r="2023" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A2023">
+        <v>2022</v>
+      </c>
+      <c r="B2023" t="s">
+        <v>2423</v>
+      </c>
+      <c r="C2023" t="s">
+        <v>1508</v>
+      </c>
+      <c r="D2023" t="s">
+        <v>2460</v>
+      </c>
+    </row>
+    <row r="2024" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A2024">
+        <v>2023</v>
+      </c>
+      <c r="B2024" t="s">
+        <v>2424</v>
+      </c>
+      <c r="C2024" t="s">
+        <v>1508</v>
+      </c>
+      <c r="D2024" t="s">
+        <v>2461</v>
+      </c>
+    </row>
+    <row r="2025" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A2025">
+        <v>2024</v>
+      </c>
+      <c r="B2025" t="s">
+        <v>2425</v>
+      </c>
+      <c r="C2025" t="s">
+        <v>1508</v>
+      </c>
+      <c r="D2025" t="s">
+        <v>2462</v>
+      </c>
+    </row>
+    <row r="2026" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A2026">
+        <v>2025</v>
+      </c>
+      <c r="B2026" t="s">
+        <v>2426</v>
+      </c>
+      <c r="C2026" t="s">
+        <v>1508</v>
+      </c>
+      <c r="D2026" t="s">
+        <v>2463</v>
+      </c>
+    </row>
+    <row r="2027" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A2027">
+        <v>2026</v>
+      </c>
+      <c r="B2027" t="s">
+        <v>2427</v>
+      </c>
+      <c r="C2027" t="s">
+        <v>1508</v>
+      </c>
+      <c r="D2027" t="s">
+        <v>2464</v>
+      </c>
+    </row>
+    <row r="2028" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A2028">
+        <v>2027</v>
+      </c>
+      <c r="B2028" t="s">
+        <v>2428</v>
+      </c>
+      <c r="C2028" t="s">
+        <v>1508</v>
+      </c>
+      <c r="D2028" t="s">
+        <v>2465</v>
+      </c>
+    </row>
+    <row r="2029" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A2029">
+        <v>2028</v>
+      </c>
+      <c r="B2029" t="s">
+        <v>2429</v>
+      </c>
+      <c r="C2029" t="s">
+        <v>1508</v>
+      </c>
+      <c r="D2029" t="s">
+        <v>2466</v>
+      </c>
+    </row>
+    <row r="2030" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A2030">
+        <v>2029</v>
+      </c>
+      <c r="B2030" t="s">
+        <v>2430</v>
+      </c>
+      <c r="C2030" t="s">
+        <v>1508</v>
+      </c>
+      <c r="D2030" t="s">
+        <v>2467</v>
+      </c>
+    </row>
+    <row r="2031" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A2031">
+        <v>2030</v>
+      </c>
+      <c r="B2031" t="s">
+        <v>2431</v>
+      </c>
+      <c r="C2031" t="s">
+        <v>1508</v>
+      </c>
+      <c r="D2031" t="s">
+        <v>2468</v>
+      </c>
+    </row>
+    <row r="2032" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A2032">
+        <v>2031</v>
+      </c>
+      <c r="B2032" t="s">
+        <v>2432</v>
+      </c>
+      <c r="C2032" t="s">
+        <v>1508</v>
+      </c>
+      <c r="D2032" t="s">
+        <v>2469</v>
+      </c>
+    </row>
+    <row r="2033" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A2033">
+        <v>2032</v>
+      </c>
+      <c r="B2033" t="s">
+        <v>2433</v>
+      </c>
+      <c r="C2033" t="s">
+        <v>1508</v>
+      </c>
+      <c r="D2033" t="s">
+        <v>2470</v>
+      </c>
+    </row>
+    <row r="2034" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A2034">
+        <v>2033</v>
+      </c>
+      <c r="B2034" t="s">
+        <v>2434</v>
+      </c>
+      <c r="C2034" t="s">
+        <v>1508</v>
+      </c>
+      <c r="D2034" t="s">
+        <v>2471</v>
+      </c>
+    </row>
+    <row r="2035" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A2035">
+        <v>2034</v>
+      </c>
+      <c r="B2035" t="s">
+        <v>2435</v>
+      </c>
+      <c r="C2035" t="s">
+        <v>1508</v>
+      </c>
+      <c r="D2035" t="s">
+        <v>2472</v>
+      </c>
+    </row>
+    <row r="2036" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A2036">
+        <v>2035</v>
+      </c>
+      <c r="B2036" t="s">
+        <v>2436</v>
+      </c>
+      <c r="C2036" t="s">
+        <v>1508</v>
+      </c>
+      <c r="D2036" t="s">
+        <v>2473</v>
+      </c>
+    </row>
+    <row r="2037" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A2037">
+        <v>2036</v>
+      </c>
+      <c r="B2037" t="s">
+        <v>2437</v>
+      </c>
+      <c r="C2037" t="s">
+        <v>1508</v>
+      </c>
+      <c r="D2037" t="s">
+        <v>2474</v>
+      </c>
+    </row>
+    <row r="2038" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A2038">
+        <v>2037</v>
+      </c>
+      <c r="B2038" t="s">
+        <v>2438</v>
+      </c>
+      <c r="C2038" t="s">
+        <v>1508</v>
+      </c>
+      <c r="D2038" t="s">
+        <v>2475</v>
+      </c>
+    </row>
+    <row r="2039" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A2039">
+        <v>2038</v>
+      </c>
+      <c r="B2039" t="s">
+        <v>2476</v>
+      </c>
+      <c r="C2039" t="s">
+        <v>503</v>
+      </c>
+      <c r="D2039" t="s">
+        <v>1507</v>
+      </c>
+    </row>
+    <row r="2040" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A2040">
+        <v>2039</v>
+      </c>
+      <c r="B2040" t="s">
+        <v>2477</v>
+      </c>
+      <c r="C2040" t="s">
+        <v>503</v>
+      </c>
+      <c r="D2040" t="s">
+        <v>1507</v>
+      </c>
+    </row>
+    <row r="2041" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A2041">
+        <v>2040</v>
+      </c>
+      <c r="B2041" t="s">
+        <v>2478</v>
+      </c>
+      <c r="C2041" t="s">
+        <v>503</v>
+      </c>
+      <c r="D2041" t="s">
+        <v>1507</v>
+      </c>
+    </row>
+    <row r="2042" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A2042">
+        <v>2041</v>
+      </c>
+      <c r="B2042" t="s">
+        <v>2479</v>
+      </c>
+      <c r="C2042" t="s">
+        <v>503</v>
+      </c>
+      <c r="D2042" t="s">
+        <v>1507</v>
+      </c>
+    </row>
+    <row r="2043" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A2043">
+        <v>2042</v>
+      </c>
+      <c r="B2043" t="s">
+        <v>2480</v>
+      </c>
+      <c r="C2043" t="s">
+        <v>503</v>
+      </c>
+      <c r="D2043" t="s">
+        <v>1507</v>
+      </c>
+    </row>
+    <row r="2044" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A2044">
+        <v>2043</v>
+      </c>
+      <c r="B2044" t="s">
+        <v>2481</v>
+      </c>
+      <c r="C2044" t="s">
+        <v>503</v>
+      </c>
+      <c r="D2044" t="s">
+        <v>1507</v>
+      </c>
+    </row>
+    <row r="2045" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A2045">
+        <v>2044</v>
+      </c>
+      <c r="B2045" t="s">
+        <v>2482</v>
+      </c>
+      <c r="C2045" t="s">
+        <v>503</v>
+      </c>
+      <c r="D2045" t="s">
+        <v>1507</v>
+      </c>
+    </row>
+    <row r="2046" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A2046">
+        <v>2045</v>
+      </c>
+      <c r="B2046" t="s">
+        <v>2483</v>
+      </c>
+      <c r="C2046" t="s">
+        <v>503</v>
+      </c>
+      <c r="D2046" t="s">
+        <v>1507</v>
+      </c>
+    </row>
+    <row r="2047" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A2047">
+        <v>2046</v>
+      </c>
+      <c r="B2047" t="s">
+        <v>2484</v>
+      </c>
+      <c r="C2047" t="s">
+        <v>503</v>
+      </c>
+      <c r="D2047" t="s">
+        <v>1507</v>
+      </c>
+    </row>
+    <row r="2048" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A2048">
+        <v>2047</v>
+      </c>
+      <c r="B2048" t="s">
+        <v>2485</v>
+      </c>
+      <c r="C2048" t="s">
+        <v>503</v>
+      </c>
+      <c r="D2048" t="s">
+        <v>1507</v>
+      </c>
+    </row>
+    <row r="2049" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A2049">
+        <v>2048</v>
+      </c>
+      <c r="B2049" t="s">
+        <v>2486</v>
+      </c>
+      <c r="C2049" t="s">
+        <v>503</v>
+      </c>
+      <c r="D2049" t="s">
+        <v>1507</v>
+      </c>
+    </row>
+    <row r="2050" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A2050">
+        <v>2049</v>
+      </c>
+      <c r="B2050" t="s">
+        <v>2487</v>
+      </c>
+      <c r="C2050" t="s">
+        <v>503</v>
+      </c>
+      <c r="D2050" t="s">
+        <v>1507</v>
+      </c>
+    </row>
+    <row r="2051" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A2051">
+        <v>2050</v>
+      </c>
+      <c r="B2051" t="s">
+        <v>2488</v>
+      </c>
+      <c r="C2051" t="s">
+        <v>503</v>
+      </c>
+      <c r="D2051" t="s">
+        <v>1507</v>
+      </c>
+    </row>
+    <row r="2052" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A2052">
+        <v>2051</v>
+      </c>
+      <c r="B2052" t="s">
+        <v>2489</v>
+      </c>
+      <c r="C2052" t="s">
+        <v>503</v>
+      </c>
+      <c r="D2052" t="s">
+        <v>1507</v>
+      </c>
+    </row>
+    <row r="2053" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A2053">
+        <v>2052</v>
+      </c>
+      <c r="B2053" t="s">
+        <v>2490</v>
+      </c>
+      <c r="C2053" t="s">
+        <v>503</v>
+      </c>
+      <c r="D2053" t="s">
+        <v>1507</v>
+      </c>
+    </row>
+    <row r="2054" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A2054">
+        <v>2053</v>
+      </c>
+      <c r="B2054" t="s">
+        <v>2491</v>
+      </c>
+      <c r="C2054" t="s">
+        <v>503</v>
+      </c>
+      <c r="D2054" t="s">
+        <v>1507</v>
+      </c>
+    </row>
+    <row r="2055" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A2055">
+        <v>2054</v>
+      </c>
+      <c r="B2055" t="s">
+        <v>2492</v>
+      </c>
+      <c r="C2055" t="s">
+        <v>503</v>
+      </c>
+      <c r="D2055" t="s">
+        <v>1507</v>
+      </c>
+    </row>
+    <row r="2056" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A2056">
+        <v>2055</v>
+      </c>
+      <c r="B2056" t="s">
+        <v>2493</v>
+      </c>
+      <c r="C2056" t="s">
+        <v>503</v>
+      </c>
+      <c r="D2056" t="s">
+        <v>1507</v>
+      </c>
+    </row>
+    <row r="2057" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A2057">
+        <v>2056</v>
+      </c>
+      <c r="B2057" t="s">
+        <v>2494</v>
+      </c>
+      <c r="C2057" t="s">
+        <v>503</v>
+      </c>
+      <c r="D2057" t="s">
+        <v>1507</v>
+      </c>
+    </row>
+    <row r="2058" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A2058">
+        <v>2057</v>
+      </c>
+      <c r="B2058" t="s">
+        <v>2495</v>
+      </c>
+      <c r="C2058" t="s">
+        <v>503</v>
+      </c>
+      <c r="D2058" t="s">
+        <v>1507</v>
+      </c>
+    </row>
+    <row r="2059" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A2059">
+        <v>2058</v>
+      </c>
+      <c r="B2059" t="s">
+        <v>2496</v>
+      </c>
+      <c r="C2059" t="s">
+        <v>503</v>
+      </c>
+      <c r="D2059" t="s">
+        <v>1507</v>
+      </c>
+    </row>
+    <row r="2060" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A2060">
+        <v>2059</v>
+      </c>
+      <c r="B2060" t="s">
+        <v>2497</v>
+      </c>
+      <c r="C2060" t="s">
+        <v>503</v>
+      </c>
+      <c r="D2060" t="s">
+        <v>1507</v>
+      </c>
+    </row>
+    <row r="2061" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A2061">
+        <v>2060</v>
+      </c>
+      <c r="B2061" t="s">
+        <v>2498</v>
+      </c>
+      <c r="C2061" t="s">
+        <v>503</v>
+      </c>
+      <c r="D2061" t="s">
+        <v>1507</v>
+      </c>
+    </row>
+    <row r="2062" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A2062">
+        <v>2061</v>
+      </c>
+      <c r="B2062" t="s">
+        <v>2499</v>
+      </c>
+      <c r="C2062" t="s">
+        <v>503</v>
+      </c>
+      <c r="D2062" t="s">
+        <v>1507</v>
+      </c>
+    </row>
+    <row r="2063" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A2063">
+        <v>2062</v>
+      </c>
+      <c r="B2063" t="s">
+        <v>2500</v>
+      </c>
+      <c r="C2063" t="s">
+        <v>503</v>
+      </c>
+      <c r="D2063" t="s">
+        <v>1507</v>
+      </c>
+    </row>
+    <row r="2064" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A2064">
+        <v>2063</v>
+      </c>
+      <c r="B2064" t="s">
+        <v>2501</v>
+      </c>
+      <c r="C2064" t="s">
+        <v>503</v>
+      </c>
+      <c r="D2064" t="s">
+        <v>1507</v>
+      </c>
+    </row>
+    <row r="2065" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A2065">
+        <v>2064</v>
+      </c>
+      <c r="B2065" t="s">
+        <v>2502</v>
+      </c>
+      <c r="C2065" t="s">
+        <v>503</v>
+      </c>
+      <c r="D2065" t="s">
+        <v>1507</v>
+      </c>
+    </row>
+    <row r="2066" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A2066">
+        <v>2065</v>
+      </c>
+      <c r="B2066" t="s">
+        <v>2503</v>
+      </c>
+      <c r="C2066" t="s">
+        <v>503</v>
+      </c>
+      <c r="D2066" t="s">
+        <v>1507</v>
+      </c>
+    </row>
+    <row r="2067" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A2067">
+        <v>2066</v>
+      </c>
+      <c r="B2067" t="s">
+        <v>2504</v>
+      </c>
+      <c r="C2067" t="s">
+        <v>503</v>
+      </c>
+      <c r="D2067" t="s">
+        <v>1507</v>
+      </c>
+    </row>
+    <row r="2068" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A2068">
+        <v>2067</v>
+      </c>
+      <c r="B2068" t="s">
+        <v>2505</v>
+      </c>
+      <c r="C2068" t="s">
+        <v>503</v>
+      </c>
+      <c r="D2068" t="s">
+        <v>1507</v>
+      </c>
+    </row>
+    <row r="2069" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A2069">
+        <v>2068</v>
+      </c>
+      <c r="B2069" t="s">
+        <v>2506</v>
+      </c>
+      <c r="C2069" t="s">
+        <v>503</v>
+      </c>
+      <c r="D2069" t="s">
+        <v>1507</v>
+      </c>
+    </row>
+    <row r="2070" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A2070">
+        <v>2069</v>
+      </c>
+      <c r="B2070" t="s">
+        <v>2507</v>
+      </c>
+      <c r="C2070" t="s">
+        <v>503</v>
+      </c>
+      <c r="D2070" t="s">
+        <v>1507</v>
+      </c>
+    </row>
+    <row r="2071" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A2071">
+        <v>2070</v>
+      </c>
+      <c r="B2071" t="s">
+        <v>2508</v>
+      </c>
+      <c r="C2071" t="s">
+        <v>503</v>
+      </c>
+      <c r="D2071" t="s">
+        <v>1507</v>
+      </c>
+    </row>
+    <row r="2072" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A2072">
+        <v>2071</v>
+      </c>
+      <c r="B2072" t="s">
+        <v>2509</v>
+      </c>
+      <c r="C2072" t="s">
+        <v>503</v>
+      </c>
+      <c r="D2072" t="s">
+        <v>1507</v>
+      </c>
+    </row>
+    <row r="2073" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A2073">
+        <v>2072</v>
+      </c>
+      <c r="B2073" t="s">
+        <v>2510</v>
+      </c>
+      <c r="C2073" t="s">
+        <v>503</v>
+      </c>
+      <c r="D2073" t="s">
+        <v>1507</v>
+      </c>
+    </row>
+    <row r="2074" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A2074">
+        <v>2073</v>
+      </c>
+      <c r="B2074" t="s">
+        <v>2511</v>
+      </c>
+      <c r="C2074" t="s">
+        <v>503</v>
+      </c>
+      <c r="D2074" t="s">
+        <v>1507</v>
+      </c>
+    </row>
+    <row r="2075" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A2075">
+        <v>2074</v>
+      </c>
+      <c r="B2075" t="s">
+        <v>2512</v>
+      </c>
+      <c r="C2075" t="s">
+        <v>503</v>
+      </c>
+      <c r="D2075" t="s">
+        <v>1507</v>
+      </c>
+    </row>
+    <row r="2076" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A2076">
+        <v>2075</v>
+      </c>
+      <c r="B2076" t="s">
+        <v>2513</v>
+      </c>
+      <c r="C2076" t="s">
+        <v>503</v>
+      </c>
+      <c r="D2076" t="s">
+        <v>1507</v>
+      </c>
+    </row>
+    <row r="2077" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A2077">
+        <v>2076</v>
+      </c>
+      <c r="B2077" t="s">
+        <v>2514</v>
+      </c>
+      <c r="C2077" t="s">
+        <v>503</v>
+      </c>
+      <c r="D2077" t="s">
+        <v>1507</v>
+      </c>
+    </row>
+    <row r="2078" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A2078">
+        <v>2077</v>
+      </c>
+      <c r="B2078" t="s">
+        <v>2515</v>
+      </c>
+      <c r="C2078" t="s">
+        <v>503</v>
+      </c>
+      <c r="D2078" t="s">
+        <v>1507</v>
+      </c>
+    </row>
+    <row r="2079" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A2079">
+        <v>2078</v>
+      </c>
+      <c r="B2079" t="s">
+        <v>2516</v>
+      </c>
+      <c r="C2079" t="s">
+        <v>503</v>
+      </c>
+      <c r="D2079" t="s">
+        <v>1507</v>
+      </c>
+    </row>
+    <row r="2080" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A2080">
+        <v>2079</v>
+      </c>
+      <c r="B2080" t="s">
+        <v>2517</v>
+      </c>
+      <c r="C2080" t="s">
+        <v>503</v>
+      </c>
+      <c r="D2080" t="s">
+        <v>1507</v>
+      </c>
+    </row>
+    <row r="2081" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A2081">
+        <v>2080</v>
+      </c>
+      <c r="B2081" t="s">
+        <v>2518</v>
+      </c>
+      <c r="C2081" t="s">
+        <v>503</v>
+      </c>
+      <c r="D2081" t="s">
+        <v>1507</v>
+      </c>
+    </row>
+    <row r="2082" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A2082">
+        <v>2081</v>
+      </c>
+      <c r="B2082" t="s">
+        <v>2519</v>
+      </c>
+      <c r="C2082" t="s">
+        <v>503</v>
+      </c>
+      <c r="D2082" t="s">
+        <v>1507</v>
+      </c>
+    </row>
+    <row r="2083" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A2083">
+        <v>2082</v>
+      </c>
+      <c r="B2083" t="s">
+        <v>2520</v>
+      </c>
+      <c r="C2083" t="s">
+        <v>503</v>
+      </c>
+      <c r="D2083" t="s">
+        <v>1507</v>
+      </c>
+    </row>
+    <row r="2084" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A2084">
+        <v>2083</v>
+      </c>
+      <c r="B2084" t="s">
+        <v>2521</v>
+      </c>
+      <c r="C2084" t="s">
+        <v>503</v>
+      </c>
+      <c r="D2084" t="s">
+        <v>1507</v>
+      </c>
+    </row>
+    <row r="2085" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A2085">
+        <v>2084</v>
+      </c>
+      <c r="B2085" t="s">
+        <v>2522</v>
+      </c>
+      <c r="C2085" t="s">
+        <v>503</v>
+      </c>
+      <c r="D2085" t="s">
+        <v>1507</v>
+      </c>
+    </row>
+    <row r="2086" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A2086">
+        <v>2085</v>
+      </c>
+      <c r="B2086" t="s">
+        <v>2523</v>
+      </c>
+      <c r="C2086" t="s">
+        <v>503</v>
+      </c>
+      <c r="D2086" t="s">
+        <v>1507</v>
+      </c>
+    </row>
+    <row r="2087" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A2087">
+        <v>2086</v>
+      </c>
+      <c r="B2087" t="s">
+        <v>2524</v>
+      </c>
+      <c r="C2087" t="s">
+        <v>503</v>
+      </c>
+      <c r="D2087" t="s">
+        <v>1507</v>
+      </c>
+    </row>
+    <row r="2088" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A2088">
+        <v>2087</v>
+      </c>
+      <c r="B2088" t="s">
+        <v>2525</v>
+      </c>
+      <c r="C2088" t="s">
+        <v>503</v>
+      </c>
+      <c r="D2088" t="s">
+        <v>1507</v>
+      </c>
+    </row>
+    <row r="2089" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A2089">
+        <v>2088</v>
+      </c>
+      <c r="B2089" t="s">
+        <v>2526</v>
+      </c>
+      <c r="C2089" t="s">
+        <v>1004</v>
+      </c>
+      <c r="D2089" t="s">
+        <v>1507</v>
+      </c>
+    </row>
+    <row r="2090" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A2090">
+        <v>2089</v>
+      </c>
+      <c r="B2090" t="s">
+        <v>2527</v>
+      </c>
+      <c r="C2090" t="s">
+        <v>1004</v>
+      </c>
+      <c r="D2090" t="s">
+        <v>1507</v>
+      </c>
+    </row>
+    <row r="2091" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A2091">
+        <v>2090</v>
+      </c>
+      <c r="B2091" t="s">
+        <v>2528</v>
+      </c>
+      <c r="C2091" t="s">
+        <v>1004</v>
+      </c>
+      <c r="D2091" t="s">
+        <v>1507</v>
+      </c>
+    </row>
+    <row r="2092" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A2092">
+        <v>2091</v>
+      </c>
+      <c r="B2092" t="s">
+        <v>2529</v>
+      </c>
+      <c r="C2092" t="s">
+        <v>1004</v>
+      </c>
+      <c r="D2092" t="s">
+        <v>1507</v>
+      </c>
+    </row>
+    <row r="2093" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A2093">
+        <v>2092</v>
+      </c>
+      <c r="B2093" t="s">
+        <v>2530</v>
+      </c>
+      <c r="C2093" t="s">
+        <v>1004</v>
+      </c>
+      <c r="D2093" t="s">
+        <v>1507</v>
+      </c>
+    </row>
+    <row r="2094" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A2094">
+        <v>2093</v>
+      </c>
+      <c r="B2094" t="s">
+        <v>2531</v>
+      </c>
+      <c r="C2094" t="s">
+        <v>1004</v>
+      </c>
+      <c r="D2094" t="s">
+        <v>1507</v>
+      </c>
+    </row>
+    <row r="2095" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A2095">
+        <v>2094</v>
+      </c>
+      <c r="B2095" t="s">
+        <v>2532</v>
+      </c>
+      <c r="C2095" t="s">
+        <v>1004</v>
+      </c>
+      <c r="D2095" t="s">
+        <v>1507</v>
+      </c>
+    </row>
+    <row r="2096" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A2096">
+        <v>2095</v>
+      </c>
+      <c r="B2096" t="s">
+        <v>2533</v>
+      </c>
+      <c r="C2096" t="s">
+        <v>1004</v>
+      </c>
+      <c r="D2096" t="s">
+        <v>1507</v>
+      </c>
+    </row>
+    <row r="2097" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A2097">
+        <v>2096</v>
+      </c>
+      <c r="B2097" t="s">
+        <v>2534</v>
+      </c>
+      <c r="C2097" t="s">
+        <v>1004</v>
+      </c>
+      <c r="D2097" t="s">
+        <v>1507</v>
+      </c>
+    </row>
+    <row r="2098" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A2098">
+        <v>2097</v>
+      </c>
+      <c r="B2098" t="s">
+        <v>2535</v>
+      </c>
+      <c r="C2098" t="s">
+        <v>1004</v>
+      </c>
+      <c r="D2098" t="s">
+        <v>1507</v>
+      </c>
+    </row>
+    <row r="2099" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A2099">
+        <v>2098</v>
+      </c>
+      <c r="B2099" t="s">
+        <v>2536</v>
+      </c>
+      <c r="C2099" t="s">
+        <v>1004</v>
+      </c>
+      <c r="D2099" t="s">
+        <v>1507</v>
+      </c>
+    </row>
+    <row r="2100" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A2100">
+        <v>2099</v>
+      </c>
+      <c r="B2100" t="s">
+        <v>2537</v>
+      </c>
+      <c r="C2100" t="s">
+        <v>1004</v>
+      </c>
+      <c r="D2100" t="s">
+        <v>1507</v>
+      </c>
+    </row>
+    <row r="2101" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A2101">
+        <v>2100</v>
+      </c>
+      <c r="B2101" t="s">
+        <v>2538</v>
+      </c>
+      <c r="C2101" t="s">
+        <v>1004</v>
+      </c>
+      <c r="D2101" t="s">
+        <v>1507</v>
+      </c>
+    </row>
+    <row r="2102" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A2102">
+        <v>2101</v>
+      </c>
+      <c r="B2102" t="s">
+        <v>2539</v>
+      </c>
+      <c r="C2102" t="s">
+        <v>1004</v>
+      </c>
+      <c r="D2102" t="s">
+        <v>1507</v>
+      </c>
+    </row>
+    <row r="2103" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A2103">
+        <v>2102</v>
+      </c>
+      <c r="B2103" t="s">
+        <v>2540</v>
+      </c>
+      <c r="C2103" t="s">
+        <v>1004</v>
+      </c>
+      <c r="D2103" t="s">
+        <v>1507</v>
+      </c>
+    </row>
+    <row r="2104" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A2104">
+        <v>2103</v>
+      </c>
+      <c r="B2104" t="s">
+        <v>2541</v>
+      </c>
+      <c r="C2104" t="s">
+        <v>1004</v>
+      </c>
+      <c r="D2104" t="s">
+        <v>1507</v>
+      </c>
+    </row>
+    <row r="2105" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A2105">
+        <v>2104</v>
+      </c>
+      <c r="B2105" t="s">
+        <v>2542</v>
+      </c>
+      <c r="C2105" t="s">
+        <v>1004</v>
+      </c>
+      <c r="D2105" t="s">
+        <v>1507</v>
+      </c>
+    </row>
+    <row r="2106" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A2106">
+        <v>2105</v>
+      </c>
+      <c r="B2106" t="s">
+        <v>2543</v>
+      </c>
+      <c r="C2106" t="s">
+        <v>1004</v>
+      </c>
+      <c r="D2106" t="s">
+        <v>1507</v>
+      </c>
+    </row>
+    <row r="2107" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A2107">
+        <v>2106</v>
+      </c>
+      <c r="B2107" t="s">
+        <v>2544</v>
+      </c>
+      <c r="C2107" t="s">
+        <v>1004</v>
+      </c>
+      <c r="D2107" t="s">
+        <v>1507</v>
+      </c>
+    </row>
+    <row r="2108" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A2108">
+        <v>2107</v>
+      </c>
+      <c r="B2108" t="s">
+        <v>2545</v>
+      </c>
+      <c r="C2108" t="s">
+        <v>1004</v>
+      </c>
+      <c r="D2108" t="s">
+        <v>1507</v>
+      </c>
+    </row>
+    <row r="2109" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A2109">
+        <v>2108</v>
+      </c>
+      <c r="B2109" t="s">
+        <v>2546</v>
+      </c>
+      <c r="C2109" t="s">
+        <v>1004</v>
+      </c>
+      <c r="D2109" t="s">
+        <v>1507</v>
+      </c>
+    </row>
+    <row r="2110" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A2110">
+        <v>2109</v>
+      </c>
+      <c r="B2110" t="s">
+        <v>2547</v>
+      </c>
+      <c r="C2110" t="s">
+        <v>1004</v>
+      </c>
+      <c r="D2110" t="s">
+        <v>1507</v>
+      </c>
+    </row>
+    <row r="2111" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A2111">
+        <v>2110</v>
+      </c>
+      <c r="B2111" t="s">
+        <v>2548</v>
+      </c>
+      <c r="C2111" t="s">
+        <v>1004</v>
+      </c>
+      <c r="D2111" t="s">
+        <v>1507</v>
+      </c>
+    </row>
+    <row r="2112" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A2112">
+        <v>2111</v>
+      </c>
+      <c r="B2112" t="s">
+        <v>2549</v>
+      </c>
+      <c r="C2112" t="s">
+        <v>1004</v>
+      </c>
+      <c r="D2112" t="s">
+        <v>1507</v>
+      </c>
+    </row>
+    <row r="2113" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A2113">
+        <v>2112</v>
+      </c>
+      <c r="B2113" t="s">
+        <v>2550</v>
+      </c>
+      <c r="C2113" t="s">
+        <v>1004</v>
+      </c>
+      <c r="D2113" t="s">
+        <v>1507</v>
+      </c>
+    </row>
+    <row r="2114" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A2114">
+        <v>2113</v>
+      </c>
+      <c r="B2114" t="s">
+        <v>2551</v>
+      </c>
+      <c r="C2114" t="s">
+        <v>1004</v>
+      </c>
+      <c r="D2114" t="s">
+        <v>1507</v>
+      </c>
+    </row>
+    <row r="2115" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A2115">
+        <v>2114</v>
+      </c>
+      <c r="B2115" t="s">
+        <v>2552</v>
+      </c>
+      <c r="C2115" t="s">
+        <v>1004</v>
+      </c>
+      <c r="D2115" t="s">
+        <v>1507</v>
+      </c>
+    </row>
+    <row r="2116" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A2116">
+        <v>2115</v>
+      </c>
+      <c r="B2116" t="s">
+        <v>2553</v>
+      </c>
+      <c r="C2116" t="s">
+        <v>1004</v>
+      </c>
+      <c r="D2116" t="s">
+        <v>1507</v>
+      </c>
+    </row>
+    <row r="2117" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A2117">
+        <v>2116</v>
+      </c>
+      <c r="B2117" t="s">
+        <v>2554</v>
+      </c>
+      <c r="C2117" t="s">
+        <v>1004</v>
+      </c>
+      <c r="D2117" t="s">
+        <v>1507</v>
+      </c>
+    </row>
+    <row r="2118" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A2118">
+        <v>2117</v>
+      </c>
+      <c r="B2118" t="s">
+        <v>2555</v>
+      </c>
+      <c r="C2118" t="s">
+        <v>1004</v>
+      </c>
+      <c r="D2118" t="s">
+        <v>1507</v>
+      </c>
+    </row>
+    <row r="2119" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A2119">
+        <v>2118</v>
+      </c>
+      <c r="B2119" t="s">
+        <v>2556</v>
+      </c>
+      <c r="C2119" t="s">
+        <v>1004</v>
+      </c>
+      <c r="D2119" t="s">
+        <v>1507</v>
+      </c>
+    </row>
+    <row r="2120" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A2120">
+        <v>2119</v>
+      </c>
+      <c r="B2120" t="s">
+        <v>2557</v>
+      </c>
+      <c r="C2120" t="s">
+        <v>1004</v>
+      </c>
+      <c r="D2120" t="s">
+        <v>1507</v>
+      </c>
+    </row>
+    <row r="2121" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A2121">
+        <v>2120</v>
+      </c>
+      <c r="B2121" t="s">
+        <v>2558</v>
+      </c>
+      <c r="C2121" t="s">
+        <v>1004</v>
+      </c>
+      <c r="D2121" t="s">
+        <v>1507</v>
+      </c>
+    </row>
+    <row r="2122" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A2122">
+        <v>2121</v>
+      </c>
+      <c r="B2122" t="s">
+        <v>2559</v>
+      </c>
+      <c r="C2122" t="s">
+        <v>1004</v>
+      </c>
+      <c r="D2122" t="s">
+        <v>1507</v>
+      </c>
+    </row>
+    <row r="2123" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A2123">
+        <v>2122</v>
+      </c>
+      <c r="B2123" t="s">
+        <v>2560</v>
+      </c>
+      <c r="C2123" t="s">
+        <v>1004</v>
+      </c>
+      <c r="D2123" t="s">
+        <v>1507</v>
+      </c>
+    </row>
+    <row r="2124" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A2124">
+        <v>2123</v>
+      </c>
+      <c r="B2124" t="s">
+        <v>2561</v>
+      </c>
+      <c r="C2124" t="s">
+        <v>1004</v>
+      </c>
+      <c r="D2124" t="s">
+        <v>1507</v>
+      </c>
+    </row>
+    <row r="2125" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A2125">
+        <v>2124</v>
+      </c>
+      <c r="B2125" t="s">
+        <v>2562</v>
+      </c>
+      <c r="C2125" t="s">
+        <v>1004</v>
+      </c>
+      <c r="D2125" t="s">
+        <v>1507</v>
+      </c>
+    </row>
+    <row r="2126" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A2126">
+        <v>2125</v>
+      </c>
+      <c r="B2126" t="s">
+        <v>2563</v>
+      </c>
+      <c r="C2126" t="s">
+        <v>1004</v>
+      </c>
+      <c r="D2126" t="s">
+        <v>1507</v>
+      </c>
+    </row>
+    <row r="2127" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A2127">
+        <v>2126</v>
+      </c>
+      <c r="B2127" t="s">
+        <v>2564</v>
+      </c>
+      <c r="C2127" t="s">
+        <v>1004</v>
+      </c>
+      <c r="D2127" t="s">
+        <v>1507</v>
+      </c>
+    </row>
+    <row r="2128" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A2128">
+        <v>2127</v>
+      </c>
+      <c r="B2128" t="s">
+        <v>2565</v>
+      </c>
+      <c r="C2128" t="s">
+        <v>1004</v>
+      </c>
+      <c r="D2128" t="s">
+        <v>1507</v>
+      </c>
+    </row>
+    <row r="2129" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A2129">
+        <v>2128</v>
+      </c>
+      <c r="B2129" t="s">
+        <v>2566</v>
+      </c>
+      <c r="C2129" t="s">
+        <v>1004</v>
+      </c>
+      <c r="D2129" t="s">
+        <v>1507</v>
+      </c>
+    </row>
+    <row r="2130" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A2130">
+        <v>2129</v>
+      </c>
+      <c r="B2130" t="s">
+        <v>2567</v>
+      </c>
+      <c r="C2130" t="s">
+        <v>1004</v>
+      </c>
+      <c r="D2130" t="s">
+        <v>1507</v>
+      </c>
+    </row>
+    <row r="2131" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A2131">
+        <v>2130</v>
+      </c>
+      <c r="B2131" t="s">
+        <v>2568</v>
+      </c>
+      <c r="C2131" t="s">
+        <v>1004</v>
+      </c>
+      <c r="D2131" t="s">
+        <v>1507</v>
+      </c>
+    </row>
+    <row r="2132" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A2132">
+        <v>2131</v>
+      </c>
+      <c r="B2132" t="s">
+        <v>2569</v>
+      </c>
+      <c r="C2132" t="s">
+        <v>1004</v>
+      </c>
+      <c r="D2132" t="s">
+        <v>1507</v>
+      </c>
+    </row>
+    <row r="2133" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A2133">
+        <v>2132</v>
+      </c>
+      <c r="B2133" t="s">
+        <v>2570</v>
+      </c>
+      <c r="C2133" t="s">
+        <v>1004</v>
+      </c>
+      <c r="D2133" t="s">
+        <v>1507</v>
+      </c>
+    </row>
+    <row r="2134" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A2134">
+        <v>2133</v>
+      </c>
+      <c r="B2134" t="s">
+        <v>2571</v>
+      </c>
+      <c r="C2134" t="s">
+        <v>1004</v>
+      </c>
+      <c r="D2134" t="s">
+        <v>1507</v>
+      </c>
+    </row>
+    <row r="2135" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A2135">
+        <v>2134</v>
+      </c>
+      <c r="B2135" t="s">
+        <v>2572</v>
+      </c>
+      <c r="C2135" t="s">
+        <v>1004</v>
+      </c>
+      <c r="D2135" t="s">
+        <v>1507</v>
+      </c>
+    </row>
+    <row r="2136" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A2136">
+        <v>2135</v>
+      </c>
+      <c r="B2136" t="s">
+        <v>2573</v>
+      </c>
+      <c r="C2136" t="s">
+        <v>1004</v>
+      </c>
+      <c r="D2136" t="s">
+        <v>1507</v>
+      </c>
+    </row>
+    <row r="2137" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A2137">
+        <v>2136</v>
+      </c>
+      <c r="B2137" t="s">
+        <v>2574</v>
+      </c>
+      <c r="C2137" t="s">
+        <v>1004</v>
+      </c>
+      <c r="D2137" t="s">
+        <v>1507</v>
+      </c>
+    </row>
+    <row r="2138" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A2138">
+        <v>2137</v>
+      </c>
+      <c r="B2138" t="s">
+        <v>2575</v>
+      </c>
+      <c r="C2138" t="s">
+        <v>1004</v>
+      </c>
+      <c r="D2138" t="s">
+        <v>1507</v>
+      </c>
+    </row>
+    <row r="2139" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A2139">
+        <v>2138</v>
+      </c>
+      <c r="B2139" t="s">
+        <v>2576</v>
+      </c>
+      <c r="C2139" t="s">
+        <v>1505</v>
+      </c>
+      <c r="D2139" t="s">
+        <v>1507</v>
+      </c>
+    </row>
+    <row r="2140" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A2140">
+        <v>2139</v>
+      </c>
+      <c r="B2140" t="s">
+        <v>2577</v>
+      </c>
+      <c r="C2140" t="s">
+        <v>1505</v>
+      </c>
+      <c r="D2140" t="s">
+        <v>1507</v>
+      </c>
+    </row>
+    <row r="2141" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A2141">
+        <v>2140</v>
+      </c>
+      <c r="B2141" t="s">
+        <v>2578</v>
+      </c>
+      <c r="C2141" t="s">
+        <v>1505</v>
+      </c>
+      <c r="D2141" t="s">
+        <v>1507</v>
+      </c>
+    </row>
+    <row r="2142" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A2142">
+        <v>2141</v>
+      </c>
+      <c r="B2142" t="s">
+        <v>2579</v>
+      </c>
+      <c r="C2142" t="s">
+        <v>1505</v>
+      </c>
+      <c r="D2142" t="s">
+        <v>1507</v>
+      </c>
+    </row>
+    <row r="2143" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A2143">
+        <v>2142</v>
+      </c>
+      <c r="B2143" t="s">
+        <v>2580</v>
+      </c>
+      <c r="C2143" t="s">
+        <v>1505</v>
+      </c>
+      <c r="D2143" t="s">
+        <v>1507</v>
+      </c>
+    </row>
+    <row r="2144" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A2144">
+        <v>2143</v>
+      </c>
+      <c r="B2144" t="s">
+        <v>2581</v>
+      </c>
+      <c r="C2144" t="s">
+        <v>1505</v>
+      </c>
+      <c r="D2144" t="s">
+        <v>1507</v>
+      </c>
+    </row>
+    <row r="2145" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A2145">
+        <v>2144</v>
+      </c>
+      <c r="B2145" t="s">
+        <v>2582</v>
+      </c>
+      <c r="C2145" t="s">
+        <v>1505</v>
+      </c>
+      <c r="D2145" t="s">
+        <v>1507</v>
+      </c>
+    </row>
+    <row r="2146" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A2146">
+        <v>2145</v>
+      </c>
+      <c r="B2146" t="s">
+        <v>2583</v>
+      </c>
+      <c r="C2146" t="s">
+        <v>1505</v>
+      </c>
+      <c r="D2146" t="s">
+        <v>1507</v>
+      </c>
+    </row>
+    <row r="2147" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A2147">
+        <v>2146</v>
+      </c>
+      <c r="B2147" t="s">
+        <v>2584</v>
+      </c>
+      <c r="C2147" t="s">
+        <v>1505</v>
+      </c>
+      <c r="D2147" t="s">
+        <v>1507</v>
+      </c>
+    </row>
+    <row r="2148" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A2148">
+        <v>2147</v>
+      </c>
+      <c r="B2148" t="s">
+        <v>2585</v>
+      </c>
+      <c r="C2148" t="s">
+        <v>1505</v>
+      </c>
+      <c r="D2148" t="s">
+        <v>1507</v>
+      </c>
+    </row>
+    <row r="2149" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A2149">
+        <v>2148</v>
+      </c>
+      <c r="B2149" t="s">
+        <v>2586</v>
+      </c>
+      <c r="C2149" t="s">
+        <v>1505</v>
+      </c>
+      <c r="D2149" t="s">
+        <v>1507</v>
+      </c>
+    </row>
+    <row r="2150" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A2150">
+        <v>2149</v>
+      </c>
+      <c r="B2150" t="s">
+        <v>2587</v>
+      </c>
+      <c r="C2150" t="s">
+        <v>1505</v>
+      </c>
+      <c r="D2150" t="s">
+        <v>1507</v>
+      </c>
+    </row>
+    <row r="2151" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A2151">
+        <v>2150</v>
+      </c>
+      <c r="B2151" t="s">
+        <v>2588</v>
+      </c>
+      <c r="C2151" t="s">
+        <v>1505</v>
+      </c>
+      <c r="D2151" t="s">
+        <v>1507</v>
+      </c>
+    </row>
+    <row r="2152" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A2152">
+        <v>2151</v>
+      </c>
+      <c r="B2152" t="s">
+        <v>2589</v>
+      </c>
+      <c r="C2152" t="s">
+        <v>1505</v>
+      </c>
+      <c r="D2152" t="s">
+        <v>1507</v>
+      </c>
+    </row>
+    <row r="2153" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A2153">
+        <v>2152</v>
+      </c>
+      <c r="B2153" t="s">
+        <v>2590</v>
+      </c>
+      <c r="C2153" t="s">
+        <v>1505</v>
+      </c>
+      <c r="D2153" t="s">
+        <v>1507</v>
+      </c>
+    </row>
+    <row r="2154" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A2154">
+        <v>2153</v>
+      </c>
+      <c r="B2154" t="s">
+        <v>2591</v>
+      </c>
+      <c r="C2154" t="s">
+        <v>1505</v>
+      </c>
+      <c r="D2154" t="s">
+        <v>1507</v>
+      </c>
+    </row>
+    <row r="2155" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A2155">
+        <v>2154</v>
+      </c>
+      <c r="B2155" t="s">
+        <v>2592</v>
+      </c>
+      <c r="C2155" t="s">
+        <v>1505</v>
+      </c>
+      <c r="D2155" t="s">
+        <v>1507</v>
+      </c>
+    </row>
+    <row r="2156" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A2156">
+        <v>2155</v>
+      </c>
+      <c r="B2156" t="s">
+        <v>2593</v>
+      </c>
+      <c r="C2156" t="s">
+        <v>1505</v>
+      </c>
+      <c r="D2156" t="s">
+        <v>1507</v>
+      </c>
+    </row>
+    <row r="2157" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A2157">
+        <v>2156</v>
+      </c>
+      <c r="B2157" t="s">
+        <v>2594</v>
+      </c>
+      <c r="C2157" t="s">
+        <v>1505</v>
+      </c>
+      <c r="D2157" t="s">
+        <v>1507</v>
+      </c>
+    </row>
+    <row r="2158" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A2158">
+        <v>2157</v>
+      </c>
+      <c r="B2158" t="s">
+        <v>2595</v>
+      </c>
+      <c r="C2158" t="s">
+        <v>1505</v>
+      </c>
+      <c r="D2158" t="s">
+        <v>1507</v>
+      </c>
+    </row>
+    <row r="2159" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A2159">
+        <v>2158</v>
+      </c>
+      <c r="B2159" t="s">
+        <v>2596</v>
+      </c>
+      <c r="C2159" t="s">
+        <v>1505</v>
+      </c>
+      <c r="D2159" t="s">
+        <v>1507</v>
+      </c>
+    </row>
+    <row r="2160" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A2160">
+        <v>2159</v>
+      </c>
+      <c r="B2160" t="s">
+        <v>2597</v>
+      </c>
+      <c r="C2160" t="s">
+        <v>1505</v>
+      </c>
+      <c r="D2160" t="s">
+        <v>1507</v>
+      </c>
+    </row>
+    <row r="2161" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A2161">
+        <v>2160</v>
+      </c>
+      <c r="B2161" t="s">
+        <v>2598</v>
+      </c>
+      <c r="C2161" t="s">
+        <v>1505</v>
+      </c>
+      <c r="D2161" t="s">
+        <v>1507</v>
+      </c>
+    </row>
+    <row r="2162" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A2162">
+        <v>2161</v>
+      </c>
+      <c r="B2162" t="s">
+        <v>2599</v>
+      </c>
+      <c r="C2162" t="s">
+        <v>1505</v>
+      </c>
+      <c r="D2162" t="s">
+        <v>1507</v>
+      </c>
+    </row>
+    <row r="2163" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A2163">
+        <v>2162</v>
+      </c>
+      <c r="B2163" t="s">
+        <v>2600</v>
+      </c>
+      <c r="C2163" t="s">
+        <v>1505</v>
+      </c>
+      <c r="D2163" t="s">
+        <v>1507</v>
+      </c>
+    </row>
+    <row r="2164" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A2164">
+        <v>2163</v>
+      </c>
+      <c r="B2164" t="s">
+        <v>2601</v>
+      </c>
+      <c r="C2164" t="s">
+        <v>1505</v>
+      </c>
+      <c r="D2164" t="s">
+        <v>1507</v>
+      </c>
+    </row>
+    <row r="2165" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A2165">
+        <v>2164</v>
+      </c>
+      <c r="B2165" t="s">
+        <v>2602</v>
+      </c>
+      <c r="C2165" t="s">
+        <v>1505</v>
+      </c>
+      <c r="D2165" t="s">
+        <v>1507</v>
+      </c>
+    </row>
+    <row r="2166" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A2166">
+        <v>2165</v>
+      </c>
+      <c r="B2166" t="s">
+        <v>2603</v>
+      </c>
+      <c r="C2166" t="s">
+        <v>1505</v>
+      </c>
+      <c r="D2166" t="s">
+        <v>1507</v>
+      </c>
+    </row>
+    <row r="2167" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A2167">
+        <v>2166</v>
+      </c>
+      <c r="B2167" t="s">
+        <v>2604</v>
+      </c>
+      <c r="C2167" t="s">
+        <v>1505</v>
+      </c>
+      <c r="D2167" t="s">
+        <v>1507</v>
+      </c>
+    </row>
+    <row r="2168" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A2168">
+        <v>2167</v>
+      </c>
+      <c r="B2168" t="s">
+        <v>2605</v>
+      </c>
+      <c r="C2168" t="s">
+        <v>1505</v>
+      </c>
+      <c r="D2168" t="s">
+        <v>1507</v>
+      </c>
+    </row>
+    <row r="2169" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A2169">
+        <v>2168</v>
+      </c>
+      <c r="B2169" t="s">
+        <v>2606</v>
+      </c>
+      <c r="C2169" t="s">
+        <v>1505</v>
+      </c>
+      <c r="D2169" t="s">
+        <v>1507</v>
+      </c>
+    </row>
+    <row r="2170" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A2170">
+        <v>2169</v>
+      </c>
+      <c r="B2170" t="s">
+        <v>2607</v>
+      </c>
+      <c r="C2170" t="s">
+        <v>1505</v>
+      </c>
+      <c r="D2170" t="s">
+        <v>1507</v>
+      </c>
+    </row>
+    <row r="2171" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A2171">
+        <v>2170</v>
+      </c>
+      <c r="B2171" t="s">
+        <v>2608</v>
+      </c>
+      <c r="C2171" t="s">
+        <v>1505</v>
+      </c>
+      <c r="D2171" t="s">
+        <v>1507</v>
+      </c>
+    </row>
+    <row r="2172" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A2172">
+        <v>2171</v>
+      </c>
+      <c r="B2172" t="s">
+        <v>2609</v>
+      </c>
+      <c r="C2172" t="s">
+        <v>1505</v>
+      </c>
+      <c r="D2172" t="s">
+        <v>1507</v>
+      </c>
+    </row>
+    <row r="2173" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A2173">
+        <v>2172</v>
+      </c>
+      <c r="B2173" t="s">
+        <v>2610</v>
+      </c>
+      <c r="C2173" t="s">
+        <v>1505</v>
+      </c>
+      <c r="D2173" t="s">
+        <v>1507</v>
+      </c>
+    </row>
+    <row r="2174" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A2174">
+        <v>2173</v>
+      </c>
+      <c r="B2174" t="s">
+        <v>2611</v>
+      </c>
+      <c r="C2174" t="s">
+        <v>1505</v>
+      </c>
+      <c r="D2174" t="s">
+        <v>1507</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>